<commit_message>
Update PODCAT-726 feature: remove PGDI from Elasticsearch index for documentation search
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\floresjimenezrh\Desktop\CCDC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuw5/Documents/GitHub/CCDC-ETL/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E52AFEC6-E054-4B20-83AC-EA408C3F0A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A9FDA8-2002-9A47-87E4-ADAB43544338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="31040" windowHeight="16540" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Site glossary'!$A$1:$Z$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Site glossary'!$A$1:$Z$58</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="188">
   <si>
     <t>Term Category</t>
   </si>
@@ -368,12 +368,6 @@
   </si>
   <si>
     <t>Pediatric Molecular Analysis for Therapy Choice</t>
-  </si>
-  <si>
-    <t>PGDI</t>
-  </si>
-  <si>
-    <t>Pediatric Genomic Data Inventory</t>
   </si>
   <si>
     <t>PPTC</t>
@@ -614,7 +608,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1020,23 +1014,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="99.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="97.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="39.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="99.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="97.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1053,7 +1047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1070,7 +1064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1081,7 +1075,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29.1">
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1098,7 +1092,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1115,7 +1109,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1132,7 +1126,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5">
+    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1143,7 +1137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29.1">
+    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1154,7 +1148,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1171,7 +1165,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -1182,7 +1176,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1193,7 +1187,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1204,7 +1198,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1215,7 +1209,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1226,7 +1220,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1237,7 +1231,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1248,7 +1242,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1259,7 +1253,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1270,7 +1264,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1281,7 +1275,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -1292,7 +1286,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1303,7 +1297,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1314,7 +1308,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1325,7 +1319,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
@@ -1336,7 +1330,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>59</v>
       </c>
@@ -1347,7 +1341,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1364,7 +1358,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1381,7 +1375,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1392,7 +1386,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="43.5">
+    <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1403,7 +1397,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="29.1">
+    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
@@ -1420,7 +1414,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="57.95">
+    <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -1437,7 +1431,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="43.5">
+    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>80</v>
       </c>
@@ -1448,7 +1442,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="29.1">
+    <row r="33" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
@@ -1459,7 +1453,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>85</v>
       </c>
@@ -1470,7 +1464,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>85</v>
       </c>
@@ -1481,7 +1475,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>85</v>
       </c>
@@ -1492,7 +1486,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
@@ -1503,7 +1497,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>85</v>
       </c>
@@ -1514,7 +1508,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1525,7 +1519,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
@@ -1536,7 +1530,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1547,7 +1541,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>85</v>
       </c>
@@ -1558,7 +1552,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>85</v>
       </c>
@@ -1569,7 +1563,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
@@ -1580,7 +1574,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>85</v>
       </c>
@@ -1591,7 +1585,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>85</v>
       </c>
@@ -1602,7 +1596,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>85</v>
       </c>
@@ -1613,7 +1607,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>85</v>
       </c>
@@ -1624,7 +1618,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>85</v>
       </c>
@@ -1635,7 +1629,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>85</v>
       </c>
@@ -1646,7 +1640,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
@@ -1657,7 +1651,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>85</v>
       </c>
@@ -1668,29 +1662,29 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>124</v>
+        <v>5</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="29.1">
+    <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="29.1">
+    <row r="55" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>126</v>
       </c>
@@ -1700,44 +1694,44 @@
       <c r="C55" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="72.599999999999994">
+      <c r="D55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="29.1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E57" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="72.599999999999994">
+    <row r="58" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>138</v>
@@ -1746,9 +1740,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="87">
+    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>140</v>
@@ -1757,7 +1751,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>85</v>
       </c>
@@ -1768,7 +1762,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>85</v>
       </c>
@@ -1779,7 +1773,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>85</v>
       </c>
@@ -1790,7 +1784,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>85</v>
       </c>
@@ -1801,9 +1795,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>150</v>
@@ -1812,9 +1806,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>152</v>
@@ -1823,9 +1817,9 @@
         <v>153</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>154</v>
@@ -1834,7 +1828,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>30</v>
       </c>
@@ -1845,18 +1839,18 @@
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>30</v>
       </c>
@@ -1867,7 +1861,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>30</v>
       </c>
@@ -1878,7 +1872,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>30</v>
       </c>
@@ -1889,7 +1883,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>30</v>
       </c>
@@ -1900,9 +1894,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>168</v>
@@ -1911,29 +1905,29 @@
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15">
-      <c r="A74" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B74" s="1" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" t="s">
         <v>170</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15">
+    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>30</v>
       </c>
       <c r="B75" t="s">
         <v>172</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="6" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15">
+    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>30</v>
       </c>
@@ -1944,7 +1938,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15">
+    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>30</v>
       </c>
@@ -1955,7 +1949,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15">
+    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>30</v>
       </c>
@@ -1966,18 +1960,18 @@
         <v>179</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15">
-      <c r="A79" t="s">
-        <v>30</v>
-      </c>
-      <c r="B79" t="s">
+    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C79" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15">
+    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>85</v>
       </c>
@@ -1988,43 +1982,32 @@
         <v>183</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15">
+    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="8" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="B82" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C82" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15">
-      <c r="A83" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>189</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:Z59" xr:uid="{A4DAB4A1-0C2C-4B2F-A024-FF4C6E1E16D8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E59">
-      <sortCondition ref="A1:A59"/>
+  <autoFilter ref="A1:Z58" xr:uid="{A4DAB4A1-0C2C-4B2F-A024-FF4C6E1E16D8}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E58">
+      <sortCondition ref="A1:A58"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2044,6 +2027,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -2266,23 +2258,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Update PODCAT-726 feature: remove PGDI from Elasticsearch index for documentation search"
This reverts commit 30ddd020bc7f1812a960c5bdcf12ebb945908396.
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25602"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuw5/Documents/GitHub/CCDC-ETL/data_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\floresjimenezrh\Desktop\CCDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A9FDA8-2002-9A47-87E4-ADAB43544338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E52AFEC6-E054-4B20-83AC-EA408C3F0A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="31040" windowHeight="16540" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Site glossary'!$A$1:$Z$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Site glossary'!$A$1:$Z$59</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="190">
   <si>
     <t>Term Category</t>
   </si>
@@ -368,6 +368,12 @@
   </si>
   <si>
     <t>Pediatric Molecular Analysis for Therapy Choice</t>
+  </si>
+  <si>
+    <t>PGDI</t>
+  </si>
+  <si>
+    <t>Pediatric Genomic Data Inventory</t>
   </si>
   <si>
     <t>PPTC</t>
@@ -608,7 +614,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1014,23 +1020,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="99.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="97.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="39.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="99.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="97.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1075,7 +1081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="29.1">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1092,7 +1098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1109,7 +1115,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1126,7 +1132,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="43.5">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1137,7 +1143,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="29.1">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1148,7 +1154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1165,7 +1171,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -1176,7 +1182,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1187,7 +1193,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1198,7 +1204,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1209,7 +1215,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1220,7 +1226,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1242,7 +1248,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1253,7 +1259,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1264,7 +1270,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1275,7 +1281,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -1286,7 +1292,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1297,7 +1303,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1308,7 +1314,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1319,7 +1325,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
@@ -1330,7 +1336,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>59</v>
       </c>
@@ -1341,7 +1347,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1358,7 +1364,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1375,7 +1381,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1386,7 +1392,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="43.5">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1397,7 +1403,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="29.1">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
@@ -1414,7 +1420,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="57.95">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -1431,7 +1437,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="43.5">
       <c r="A32" s="1" t="s">
         <v>80</v>
       </c>
@@ -1442,7 +1448,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="29.1">
       <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
@@ -1453,7 +1459,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
         <v>85</v>
       </c>
@@ -1464,7 +1470,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
         <v>85</v>
       </c>
@@ -1475,7 +1481,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
         <v>85</v>
       </c>
@@ -1486,7 +1492,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
@@ -1497,7 +1503,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
         <v>85</v>
       </c>
@@ -1508,7 +1514,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1519,7 +1525,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
@@ -1530,7 +1536,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1541,7 +1547,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
         <v>85</v>
       </c>
@@ -1552,7 +1558,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
         <v>85</v>
       </c>
@@ -1563,7 +1569,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
@@ -1574,7 +1580,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
         <v>85</v>
       </c>
@@ -1585,7 +1591,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
         <v>85</v>
       </c>
@@ -1596,7 +1602,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
         <v>85</v>
       </c>
@@ -1607,7 +1613,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
         <v>85</v>
       </c>
@@ -1618,7 +1624,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
         <v>85</v>
       </c>
@@ -1629,7 +1635,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
         <v>85</v>
       </c>
@@ -1640,7 +1646,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
@@ -1651,7 +1657,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
         <v>85</v>
       </c>
@@ -1662,29 +1668,29 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" ht="29.1">
       <c r="A54" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" ht="29.1">
       <c r="A55" s="1" t="s">
         <v>126</v>
       </c>
@@ -1694,44 +1700,44 @@
       <c r="C55" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D55" s="1" t="s">
+    </row>
+    <row r="56" spans="1:5" ht="72.599999999999994">
+      <c r="A56" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B56" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="E56" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D56" s="1" t="s">
+    </row>
+    <row r="57" spans="1:5" ht="29.1">
+      <c r="A57" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="C57" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B57" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="E57" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="72.599999999999994">
       <c r="A58" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>138</v>
@@ -1740,9 +1746,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" ht="87">
       <c r="A59" s="1" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>140</v>
@@ -1751,7 +1757,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
         <v>85</v>
       </c>
@@ -1762,7 +1768,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
         <v>85</v>
       </c>
@@ -1773,7 +1779,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
         <v>85</v>
       </c>
@@ -1784,7 +1790,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
         <v>85</v>
       </c>
@@ -1795,9 +1801,9 @@
         <v>149</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>150</v>
@@ -1806,9 +1812,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>152</v>
@@ -1817,9 +1823,9 @@
         <v>153</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>154</v>
@@ -1828,7 +1834,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
         <v>30</v>
       </c>
@@ -1839,18 +1845,18 @@
         <v>157</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="15">
       <c r="A69" s="1" t="s">
         <v>30</v>
       </c>
@@ -1861,7 +1867,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" ht="15">
       <c r="A70" s="1" t="s">
         <v>30</v>
       </c>
@@ -1872,7 +1878,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="15">
       <c r="A71" s="1" t="s">
         <v>30</v>
       </c>
@@ -1883,7 +1889,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="15">
       <c r="A72" s="1" t="s">
         <v>30</v>
       </c>
@@ -1894,9 +1900,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" ht="15">
       <c r="A73" s="1" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>168</v>
@@ -1905,29 +1911,29 @@
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>30</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="74" spans="1:3" ht="15">
+      <c r="A74" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="15">
       <c r="A75" t="s">
         <v>30</v>
       </c>
       <c r="B75" t="s">
         <v>172</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C75" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" ht="15">
       <c r="A76" t="s">
         <v>30</v>
       </c>
@@ -1938,7 +1944,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" ht="15">
       <c r="A77" t="s">
         <v>30</v>
       </c>
@@ -1949,7 +1955,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="15">
       <c r="A78" t="s">
         <v>30</v>
       </c>
@@ -1960,18 +1966,18 @@
         <v>179</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" s="1" t="s">
+    <row r="79" spans="1:3" ht="15">
+      <c r="A79" t="s">
+        <v>30</v>
+      </c>
+      <c r="B79" t="s">
         <v>180</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="6" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="15">
       <c r="A80" s="1" t="s">
         <v>85</v>
       </c>
@@ -1982,32 +1988,43 @@
         <v>183</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="15">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B81" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C81" s="8" t="s">
+      <c r="C81" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="15">
       <c r="A82" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B82" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="C82" s="8" t="s">
         <v>187</v>
       </c>
     </row>
+    <row r="83" spans="1:3" ht="15">
+      <c r="A83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Z58" xr:uid="{A4DAB4A1-0C2C-4B2F-A024-FF4C6E1E16D8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E58">
-      <sortCondition ref="A1:A58"/>
+  <autoFilter ref="A1:Z59" xr:uid="{A4DAB4A1-0C2C-4B2F-A024-FF4C6E1E16D8}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E59">
+      <sortCondition ref="A1:A59"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2027,15 +2044,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -2258,40 +2266,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}"/>
 </file>
</xml_diff>

<commit_message>
Update PODCAT-731 feature: update term "repository" definition.
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuw5/Documents/GitHub/CCDC-ETL/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959AE3B0-395F-CE44-A85B-24A0C93BCCB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00A6F85-8808-4240-8201-122B5085700D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25760" windowHeight="18260" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
@@ -457,9 +457,6 @@
     <t>Repository</t>
   </si>
   <si>
-    <t>Biomedical data repositories accept submission of relevant data from the community to store, organize, validate, archive, preserve and distribute the data, in compliance with the FAIR Data Principles.  A system for storing multiple research artifacts, provided at least some of the research artifacts contain Individual Research Data. A data repository often contains artifacts from multiple studies. Some data repositories accept research datasets irrespective of the structure of those datasets; other data repositories require all research datasets to conform to a standard reference model.</t>
-  </si>
-  <si>
     <t>HCMI</t>
   </si>
   <si>
@@ -602,6 +599,9 @@
   </si>
   <si>
     <t>Pediatric Brain Tumor Project</t>
+  </si>
+  <si>
+    <t>Biomedical data repositories store, organize, validate, archive, preserve, and distribute data, in compliance with the FAIR Data Principles. It is a system for storing multiple research artifacts, provided at least some of the research artifacts contain Individual Research Data. A data repository often contains artifacts from multiple studies. Some data repositories accept research datasets irrespective of the structure of those datasets; other data repositories require all research datasets to conform to a standard reference model.</t>
   </si>
 </sst>
 </file>
@@ -679,27 +679,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,893 +1012,892 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="99.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="97.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="99.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5" customWidth="1"/>
+    <col min="5" max="5" width="97.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" s="1" t="s">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" s="1" t="s">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="1" t="s">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" s="1" t="s">
+      <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="1" t="s">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
         <v>104</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="A44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="A45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" t="s">
         <v>108</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="1" t="s">
+      <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" t="s">
         <v>110</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="A47" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="1" t="s">
+      <c r="A48" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" t="s">
         <v>114</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" s="1" t="s">
+      <c r="A49" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" t="s">
         <v>116</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="A50" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" t="s">
         <v>118</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" s="1" t="s">
+      <c r="A51" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" t="s">
         <v>120</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" s="1" t="s">
+      <c r="A52" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" t="s">
         <v>122</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>124</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>124</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>126</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>126</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>128</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" t="s">
         <v>130</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>126</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>132</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" t="s">
         <v>134</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>126</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>136</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>126</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>138</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C59" s="2" t="s">
+    </row>
+    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>85</v>
+      </c>
+      <c r="B60" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C60" s="2" t="s">
+    </row>
+    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C61" s="2" t="s">
+    </row>
+    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C62" s="2" t="s">
+    </row>
+    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C63" s="2" t="s">
+    </row>
+    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C64" s="2" t="s">
+    </row>
+    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C65" s="2" t="s">
+    </row>
+    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C66" s="2" t="s">
+    </row>
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C67" s="2" t="s">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" s="1" t="s">
+      <c r="C68" t="s">
         <v>158</v>
       </c>
-      <c r="C68" s="1" t="s">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" t="s">
         <v>160</v>
       </c>
-      <c r="C69" s="1" t="s">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" t="s">
         <v>162</v>
       </c>
-      <c r="C70" s="1" t="s">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" s="1" t="s">
+      <c r="C71" t="s">
         <v>164</v>
       </c>
-      <c r="C71" s="1" t="s">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" t="s">
         <v>166</v>
       </c>
-      <c r="C72" s="1" t="s">
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B73" s="1" t="s">
+      <c r="C73" t="s">
         <v>168</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1910,10 +1905,10 @@
         <v>30</v>
       </c>
       <c r="B74" t="s">
+        <v>169</v>
+      </c>
+      <c r="C74" t="s">
         <v>170</v>
-      </c>
-      <c r="C74" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1921,10 +1916,10 @@
         <v>30</v>
       </c>
       <c r="B75" t="s">
+        <v>171</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1932,10 +1927,10 @@
         <v>30</v>
       </c>
       <c r="B76" t="s">
+        <v>173</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1943,10 +1938,10 @@
         <v>30</v>
       </c>
       <c r="B77" t="s">
+        <v>175</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1954,54 +1949,54 @@
         <v>30</v>
       </c>
       <c r="B78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C78" s="6" t="s">
+    </row>
+    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B79" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C79" s="2" t="s">
+    </row>
+    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C80" s="2" t="s">
+    </row>
+    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81" s="7" t="s">
+      <c r="C81" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C81" s="8" t="s">
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" s="7" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B82" s="9" t="s">
+      <c r="C82" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2016,6 +2011,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -2238,27 +2253,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2275,23 +2289,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update PODCAT-731 feature: change the full name for KF data source
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuw5/Documents/GitHub/CCDC-ETL/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00A6F85-8808-4240-8201-122B5085700D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EA7C5B-F65A-2D4C-A3BF-4E1BDBB797AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25760" windowHeight="18260" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
@@ -331,9 +331,6 @@
     <t>KF</t>
   </si>
   <si>
-    <t>Kids First</t>
-  </si>
-  <si>
     <t>MyPart</t>
   </si>
   <si>
@@ -602,6 +599,9 @@
   </si>
   <si>
     <t>Biomedical data repositories store, organize, validate, archive, preserve, and distribute data, in compliance with the FAIR Data Principles. It is a system for storing multiple research artifacts, provided at least some of the research artifacts contain Individual Research Data. A data repository often contains artifacts from multiple studies. Some data repositories accept research datasets irrespective of the structure of those datasets; other data repositories require all research datasets to conform to a standard reference model.</t>
+  </si>
+  <si>
+    <t>Kids First Data Resource</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1511,7 +1511,7 @@
         <v>96</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>97</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1519,10 +1519,10 @@
         <v>85</v>
       </c>
       <c r="B40" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1530,10 +1530,10 @@
         <v>85</v>
       </c>
       <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1541,10 +1541,10 @@
         <v>85</v>
       </c>
       <c r="B42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1552,10 +1552,10 @@
         <v>85</v>
       </c>
       <c r="B43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1563,10 +1563,10 @@
         <v>85</v>
       </c>
       <c r="B44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1574,10 +1574,10 @@
         <v>85</v>
       </c>
       <c r="B45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1585,10 +1585,10 @@
         <v>85</v>
       </c>
       <c r="B46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1596,10 +1596,10 @@
         <v>85</v>
       </c>
       <c r="B47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1607,10 +1607,10 @@
         <v>85</v>
       </c>
       <c r="B48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1618,10 +1618,10 @@
         <v>85</v>
       </c>
       <c r="B49" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1629,10 +1629,10 @@
         <v>85</v>
       </c>
       <c r="B50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1640,10 +1640,10 @@
         <v>85</v>
       </c>
       <c r="B51" t="s">
+        <v>119</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1651,88 +1651,88 @@
         <v>85</v>
       </c>
       <c r="B52" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B54" t="s">
+        <v>125</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" t="s">
         <v>129</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>130</v>
-      </c>
-      <c r="E55" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B56" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" t="s">
         <v>133</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>134</v>
-      </c>
-      <c r="E56" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B57" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1740,10 +1740,10 @@
         <v>85</v>
       </c>
       <c r="B59" t="s">
+        <v>138</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1751,10 +1751,10 @@
         <v>85</v>
       </c>
       <c r="B60" t="s">
+        <v>140</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1762,10 +1762,10 @@
         <v>85</v>
       </c>
       <c r="B61" t="s">
+        <v>142</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1773,10 +1773,10 @@
         <v>85</v>
       </c>
       <c r="B62" t="s">
+        <v>144</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1784,10 +1784,10 @@
         <v>85</v>
       </c>
       <c r="B63" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1795,10 +1795,10 @@
         <v>30</v>
       </c>
       <c r="B64" t="s">
+        <v>148</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1806,10 +1806,10 @@
         <v>85</v>
       </c>
       <c r="B65" t="s">
+        <v>150</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1817,10 +1817,10 @@
         <v>30</v>
       </c>
       <c r="B66" t="s">
+        <v>152</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1828,10 +1828,10 @@
         <v>30</v>
       </c>
       <c r="B67" t="s">
+        <v>154</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -1839,10 +1839,10 @@
         <v>30</v>
       </c>
       <c r="B68" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" t="s">
         <v>157</v>
-      </c>
-      <c r="C68" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -1850,10 +1850,10 @@
         <v>30</v>
       </c>
       <c r="B69" t="s">
+        <v>158</v>
+      </c>
+      <c r="C69" t="s">
         <v>159</v>
-      </c>
-      <c r="C69" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -1861,10 +1861,10 @@
         <v>30</v>
       </c>
       <c r="B70" t="s">
+        <v>160</v>
+      </c>
+      <c r="C70" t="s">
         <v>161</v>
-      </c>
-      <c r="C70" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1872,10 +1872,10 @@
         <v>30</v>
       </c>
       <c r="B71" t="s">
+        <v>162</v>
+      </c>
+      <c r="C71" t="s">
         <v>163</v>
-      </c>
-      <c r="C71" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1883,10 +1883,10 @@
         <v>30</v>
       </c>
       <c r="B72" t="s">
+        <v>164</v>
+      </c>
+      <c r="C72" t="s">
         <v>165</v>
-      </c>
-      <c r="C72" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -1894,10 +1894,10 @@
         <v>85</v>
       </c>
       <c r="B73" t="s">
+        <v>166</v>
+      </c>
+      <c r="C73" t="s">
         <v>167</v>
-      </c>
-      <c r="C73" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1905,10 +1905,10 @@
         <v>30</v>
       </c>
       <c r="B74" t="s">
+        <v>168</v>
+      </c>
+      <c r="C74" t="s">
         <v>169</v>
-      </c>
-      <c r="C74" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1916,10 +1916,10 @@
         <v>30</v>
       </c>
       <c r="B75" t="s">
+        <v>170</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1927,10 +1927,10 @@
         <v>30</v>
       </c>
       <c r="B76" t="s">
+        <v>172</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1938,10 +1938,10 @@
         <v>30</v>
       </c>
       <c r="B77" t="s">
+        <v>174</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1949,10 +1949,10 @@
         <v>30</v>
       </c>
       <c r="B78" t="s">
+        <v>176</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1960,10 +1960,10 @@
         <v>85</v>
       </c>
       <c r="B79" t="s">
+        <v>178</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1971,10 +1971,10 @@
         <v>85</v>
       </c>
       <c r="B80" t="s">
+        <v>180</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1982,10 +1982,10 @@
         <v>85</v>
       </c>
       <c r="B81" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -1993,10 +1993,10 @@
         <v>85</v>
       </c>
       <c r="B82" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C82" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2011,15 +2011,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
@@ -2028,6 +2019,15 @@
     <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2254,20 +2254,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
     <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update PODCAT-756 feature: update glossary for dbGap resource
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25721"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuw5/Documents/GitHub/CCDC-ETL/data_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EA7C5B-F65A-2D4C-A3BF-4E1BDBB797AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6E007E2-8614-4B93-9A29-1005662F26A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25760" windowHeight="18260" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
@@ -31,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="204">
   <si>
     <t>Term Category</t>
   </si>
@@ -331,6 +332,9 @@
     <t>KF</t>
   </si>
   <si>
+    <t>Kids First Data Resource</t>
+  </si>
+  <si>
     <t>MyPart</t>
   </si>
   <si>
@@ -454,6 +458,9 @@
     <t>Repository</t>
   </si>
   <si>
+    <t>Biomedical data repositories store, organize, validate, archive, preserve, and distribute data, in compliance with the FAIR Data Principles. It is a system for storing multiple research artifacts, provided at least some of the research artifacts contain Individual Research Data. A data repository often contains artifacts from multiple studies. Some data repositories accept research datasets irrespective of the structure of those datasets; other data repositories require all research datasets to conform to a standard reference model.</t>
+  </si>
+  <si>
     <t>HCMI</t>
   </si>
   <si>
@@ -598,17 +605,59 @@
     <t>Pediatric Brain Tumor Project</t>
   </si>
   <si>
-    <t>Biomedical data repositories store, organize, validate, archive, preserve, and distribute data, in compliance with the FAIR Data Principles. It is a system for storing multiple research artifacts, provided at least some of the research artifacts contain Individual Research Data. A data repository often contains artifacts from multiple studies. Some data repositories accept research datasets irrespective of the structure of those datasets; other data repositories require all research datasets to conform to a standard reference model.</t>
-  </si>
-  <si>
-    <t>Kids First Data Resource</t>
+    <t>dbGaP</t>
+  </si>
+  <si>
+    <t>The database of genotypes and phenotypes</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>Osteosarcoma Genomics</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>Genomic Sequencing of Ewing's Sarcoma</t>
+  </si>
+  <si>
+    <t>RMS</t>
+  </si>
+  <si>
+    <t>Genomic Sequencing of Pediatric Rhabdomyosarcoma</t>
+  </si>
+  <si>
+    <t>CSER</t>
+  </si>
+  <si>
+    <t>University of Michigan Clinical Sequencing Exploratory Research</t>
+  </si>
+  <si>
+    <t>FL-HCC</t>
+  </si>
+  <si>
+    <t>Genomic and Transcriptomic Landscape of Fibrolamellar Hepatocellular Carcinoma</t>
+  </si>
+  <si>
+    <t>DIPG</t>
+  </si>
+  <si>
+    <t>Functionally-defined Therapeutic Targets in Diffuse Intrinsic Pontine Glioma</t>
+  </si>
+  <si>
+    <t>BASIC3</t>
+  </si>
+  <si>
+    <t>Baylor College of Medicine Advancing Sequencing in Childhood Cancer Care</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,6 +676,11 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -679,23 +733,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1010,993 +1069,1082 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="99.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5" customWidth="1"/>
-    <col min="5" max="5" width="97.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="99.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="97.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="29.1">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" ht="43.5">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" ht="29.1">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:5" ht="43.5">
+      <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:5" ht="29.1">
+      <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:5" ht="57.95">
+      <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:5" ht="43.5">
+      <c r="A32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" spans="1:3" ht="29.1">
+      <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="29.1">
+      <c r="A53" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="29.1">
+      <c r="A54" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="72.599999999999994">
+      <c r="A55" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="29.1">
+      <c r="A56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="72.599999999999994">
+      <c r="A57" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="72.599999999999994">
+      <c r="A58" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" t="s">
+        <v>170</v>
+      </c>
+      <c r="C74" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" t="s">
+        <v>174</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77" t="s">
+        <v>176</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" t="s">
+        <v>178</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" t="s">
-        <v>111</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" t="s">
-        <v>121</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>123</v>
-      </c>
-      <c r="B53" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>123</v>
-      </c>
-      <c r="B54" t="s">
-        <v>125</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>125</v>
-      </c>
-      <c r="B55" t="s">
-        <v>127</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D55" t="s">
-        <v>129</v>
-      </c>
-      <c r="E55" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>125</v>
-      </c>
-      <c r="B56" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D56" t="s">
-        <v>133</v>
-      </c>
-      <c r="E56" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>125</v>
-      </c>
-      <c r="B57" t="s">
-        <v>135</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>125</v>
-      </c>
-      <c r="B58" t="s">
-        <v>137</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" t="s">
-        <v>138</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>85</v>
-      </c>
-      <c r="B60" t="s">
-        <v>140</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>85</v>
-      </c>
-      <c r="B61" t="s">
-        <v>142</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>85</v>
-      </c>
-      <c r="B62" t="s">
-        <v>144</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>85</v>
-      </c>
-      <c r="B63" t="s">
-        <v>146</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>30</v>
-      </c>
-      <c r="B64" t="s">
-        <v>148</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>85</v>
-      </c>
-      <c r="B65" t="s">
-        <v>150</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>30</v>
-      </c>
-      <c r="B66" t="s">
-        <v>152</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>30</v>
-      </c>
-      <c r="B67" t="s">
-        <v>154</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" t="s">
-        <v>156</v>
-      </c>
-      <c r="C68" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" t="s">
-        <v>158</v>
-      </c>
-      <c r="C69" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" t="s">
-        <v>160</v>
-      </c>
-      <c r="C70" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" t="s">
-        <v>162</v>
-      </c>
-      <c r="C71" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>30</v>
-      </c>
-      <c r="B72" t="s">
-        <v>164</v>
-      </c>
-      <c r="C72" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>85</v>
-      </c>
-      <c r="B73" t="s">
-        <v>166</v>
-      </c>
-      <c r="C73" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>30</v>
-      </c>
-      <c r="B74" t="s">
-        <v>168</v>
-      </c>
-      <c r="C74" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>30</v>
-      </c>
-      <c r="B75" t="s">
-        <v>170</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>30</v>
-      </c>
-      <c r="B76" t="s">
-        <v>172</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>30</v>
-      </c>
-      <c r="B77" t="s">
-        <v>174</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>30</v>
-      </c>
-      <c r="B78" t="s">
-        <v>176</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" t="s">
-        <v>178</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>85</v>
-      </c>
-      <c r="B80" t="s">
-        <v>180</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>85</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>185</v>
+    <row r="83" spans="1:3" ht="15">
+      <c r="A83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15">
+      <c r="A84" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15">
+      <c r="A85" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15">
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15">
+      <c r="A87" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15">
+      <c r="A88" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15">
+      <c r="A89" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15">
+      <c r="A90" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2011,26 +2159,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -2253,40 +2381,34 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}"/>
 </file>
</xml_diff>

<commit_message>
Update PODCAT-756 feature: update glossary for dbGap resource (#58)
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25721"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuw5/Documents/GitHub/CCDC-ETL/data_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EA7C5B-F65A-2D4C-A3BF-4E1BDBB797AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6E007E2-8614-4B93-9A29-1005662F26A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25760" windowHeight="18260" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
@@ -31,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="204">
   <si>
     <t>Term Category</t>
   </si>
@@ -331,6 +332,9 @@
     <t>KF</t>
   </si>
   <si>
+    <t>Kids First Data Resource</t>
+  </si>
+  <si>
     <t>MyPart</t>
   </si>
   <si>
@@ -454,6 +458,9 @@
     <t>Repository</t>
   </si>
   <si>
+    <t>Biomedical data repositories store, organize, validate, archive, preserve, and distribute data, in compliance with the FAIR Data Principles. It is a system for storing multiple research artifacts, provided at least some of the research artifacts contain Individual Research Data. A data repository often contains artifacts from multiple studies. Some data repositories accept research datasets irrespective of the structure of those datasets; other data repositories require all research datasets to conform to a standard reference model.</t>
+  </si>
+  <si>
     <t>HCMI</t>
   </si>
   <si>
@@ -598,17 +605,59 @@
     <t>Pediatric Brain Tumor Project</t>
   </si>
   <si>
-    <t>Biomedical data repositories store, organize, validate, archive, preserve, and distribute data, in compliance with the FAIR Data Principles. It is a system for storing multiple research artifacts, provided at least some of the research artifacts contain Individual Research Data. A data repository often contains artifacts from multiple studies. Some data repositories accept research datasets irrespective of the structure of those datasets; other data repositories require all research datasets to conform to a standard reference model.</t>
-  </si>
-  <si>
-    <t>Kids First Data Resource</t>
+    <t>dbGaP</t>
+  </si>
+  <si>
+    <t>The database of genotypes and phenotypes</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>Osteosarcoma Genomics</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>Genomic Sequencing of Ewing's Sarcoma</t>
+  </si>
+  <si>
+    <t>RMS</t>
+  </si>
+  <si>
+    <t>Genomic Sequencing of Pediatric Rhabdomyosarcoma</t>
+  </si>
+  <si>
+    <t>CSER</t>
+  </si>
+  <si>
+    <t>University of Michigan Clinical Sequencing Exploratory Research</t>
+  </si>
+  <si>
+    <t>FL-HCC</t>
+  </si>
+  <si>
+    <t>Genomic and Transcriptomic Landscape of Fibrolamellar Hepatocellular Carcinoma</t>
+  </si>
+  <si>
+    <t>DIPG</t>
+  </si>
+  <si>
+    <t>Functionally-defined Therapeutic Targets in Diffuse Intrinsic Pontine Glioma</t>
+  </si>
+  <si>
+    <t>BASIC3</t>
+  </si>
+  <si>
+    <t>Baylor College of Medicine Advancing Sequencing in Childhood Cancer Care</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,6 +676,11 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -679,23 +733,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1010,993 +1069,1082 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="99.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5" customWidth="1"/>
-    <col min="5" max="5" width="97.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="99.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="97.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="29.1">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" ht="43.5">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" ht="29.1">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:5" ht="43.5">
+      <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:5" ht="29.1">
+      <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:5" ht="57.95">
+      <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:5" ht="43.5">
+      <c r="A32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" spans="1:3" ht="29.1">
+      <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="29.1">
+      <c r="A53" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="29.1">
+      <c r="A54" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="72.599999999999994">
+      <c r="A55" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="29.1">
+      <c r="A56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="72.599999999999994">
+      <c r="A57" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="72.599999999999994">
+      <c r="A58" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" t="s">
+        <v>170</v>
+      </c>
+      <c r="C74" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" t="s">
+        <v>174</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77" t="s">
+        <v>176</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" t="s">
+        <v>178</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" t="s">
-        <v>111</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" t="s">
-        <v>121</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>123</v>
-      </c>
-      <c r="B53" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>123</v>
-      </c>
-      <c r="B54" t="s">
-        <v>125</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>125</v>
-      </c>
-      <c r="B55" t="s">
-        <v>127</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D55" t="s">
-        <v>129</v>
-      </c>
-      <c r="E55" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>125</v>
-      </c>
-      <c r="B56" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D56" t="s">
-        <v>133</v>
-      </c>
-      <c r="E56" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>125</v>
-      </c>
-      <c r="B57" t="s">
-        <v>135</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>125</v>
-      </c>
-      <c r="B58" t="s">
-        <v>137</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" t="s">
-        <v>138</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>85</v>
-      </c>
-      <c r="B60" t="s">
-        <v>140</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>85</v>
-      </c>
-      <c r="B61" t="s">
-        <v>142</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>85</v>
-      </c>
-      <c r="B62" t="s">
-        <v>144</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>85</v>
-      </c>
-      <c r="B63" t="s">
-        <v>146</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>30</v>
-      </c>
-      <c r="B64" t="s">
-        <v>148</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>85</v>
-      </c>
-      <c r="B65" t="s">
-        <v>150</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>30</v>
-      </c>
-      <c r="B66" t="s">
-        <v>152</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>30</v>
-      </c>
-      <c r="B67" t="s">
-        <v>154</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" t="s">
-        <v>156</v>
-      </c>
-      <c r="C68" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" t="s">
-        <v>158</v>
-      </c>
-      <c r="C69" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" t="s">
-        <v>160</v>
-      </c>
-      <c r="C70" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" t="s">
-        <v>162</v>
-      </c>
-      <c r="C71" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>30</v>
-      </c>
-      <c r="B72" t="s">
-        <v>164</v>
-      </c>
-      <c r="C72" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>85</v>
-      </c>
-      <c r="B73" t="s">
-        <v>166</v>
-      </c>
-      <c r="C73" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>30</v>
-      </c>
-      <c r="B74" t="s">
-        <v>168</v>
-      </c>
-      <c r="C74" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>30</v>
-      </c>
-      <c r="B75" t="s">
-        <v>170</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>30</v>
-      </c>
-      <c r="B76" t="s">
-        <v>172</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>30</v>
-      </c>
-      <c r="B77" t="s">
-        <v>174</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>30</v>
-      </c>
-      <c r="B78" t="s">
-        <v>176</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" t="s">
-        <v>178</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>85</v>
-      </c>
-      <c r="B80" t="s">
-        <v>180</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>85</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>185</v>
+    <row r="83" spans="1:3" ht="15">
+      <c r="A83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15">
+      <c r="A84" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15">
+      <c r="A85" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15">
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15">
+      <c r="A87" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15">
+      <c r="A88" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15">
+      <c r="A89" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15">
+      <c r="A90" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2011,26 +2159,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -2253,40 +2381,34 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}"/>
 </file>
</xml_diff>

<commit_message>
Update PODCAT-756 feature: update glossary for dbGap resource (#58) (#59)
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25721"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuw5/Documents/GitHub/CCDC-ETL/data_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EA7C5B-F65A-2D4C-A3BF-4E1BDBB797AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6E007E2-8614-4B93-9A29-1005662F26A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25760" windowHeight="18260" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
@@ -31,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="204">
   <si>
     <t>Term Category</t>
   </si>
@@ -331,6 +332,9 @@
     <t>KF</t>
   </si>
   <si>
+    <t>Kids First Data Resource</t>
+  </si>
+  <si>
     <t>MyPart</t>
   </si>
   <si>
@@ -454,6 +458,9 @@
     <t>Repository</t>
   </si>
   <si>
+    <t>Biomedical data repositories store, organize, validate, archive, preserve, and distribute data, in compliance with the FAIR Data Principles. It is a system for storing multiple research artifacts, provided at least some of the research artifacts contain Individual Research Data. A data repository often contains artifacts from multiple studies. Some data repositories accept research datasets irrespective of the structure of those datasets; other data repositories require all research datasets to conform to a standard reference model.</t>
+  </si>
+  <si>
     <t>HCMI</t>
   </si>
   <si>
@@ -598,17 +605,59 @@
     <t>Pediatric Brain Tumor Project</t>
   </si>
   <si>
-    <t>Biomedical data repositories store, organize, validate, archive, preserve, and distribute data, in compliance with the FAIR Data Principles. It is a system for storing multiple research artifacts, provided at least some of the research artifacts contain Individual Research Data. A data repository often contains artifacts from multiple studies. Some data repositories accept research datasets irrespective of the structure of those datasets; other data repositories require all research datasets to conform to a standard reference model.</t>
-  </si>
-  <si>
-    <t>Kids First Data Resource</t>
+    <t>dbGaP</t>
+  </si>
+  <si>
+    <t>The database of genotypes and phenotypes</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>Osteosarcoma Genomics</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>Genomic Sequencing of Ewing's Sarcoma</t>
+  </si>
+  <si>
+    <t>RMS</t>
+  </si>
+  <si>
+    <t>Genomic Sequencing of Pediatric Rhabdomyosarcoma</t>
+  </si>
+  <si>
+    <t>CSER</t>
+  </si>
+  <si>
+    <t>University of Michigan Clinical Sequencing Exploratory Research</t>
+  </si>
+  <si>
+    <t>FL-HCC</t>
+  </si>
+  <si>
+    <t>Genomic and Transcriptomic Landscape of Fibrolamellar Hepatocellular Carcinoma</t>
+  </si>
+  <si>
+    <t>DIPG</t>
+  </si>
+  <si>
+    <t>Functionally-defined Therapeutic Targets in Diffuse Intrinsic Pontine Glioma</t>
+  </si>
+  <si>
+    <t>BASIC3</t>
+  </si>
+  <si>
+    <t>Baylor College of Medicine Advancing Sequencing in Childhood Cancer Care</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,6 +676,11 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -679,23 +733,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1010,993 +1069,1082 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="99.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5" customWidth="1"/>
-    <col min="5" max="5" width="97.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="99.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="97.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="29.1">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" ht="43.5">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" ht="29.1">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:5" ht="43.5">
+      <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:5" ht="29.1">
+      <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:5" ht="57.95">
+      <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:5" ht="43.5">
+      <c r="A32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="33" spans="1:3" ht="29.1">
+      <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="29.1">
+      <c r="A53" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="29.1">
+      <c r="A54" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="72.599999999999994">
+      <c r="A55" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="29.1">
+      <c r="A56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="72.599999999999994">
+      <c r="A57" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="72.599999999999994">
+      <c r="A58" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" t="s">
+        <v>170</v>
+      </c>
+      <c r="C74" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" t="s">
+        <v>174</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77" t="s">
+        <v>176</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" t="s">
+        <v>178</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" t="s">
-        <v>111</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" t="s">
-        <v>121</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>123</v>
-      </c>
-      <c r="B53" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>123</v>
-      </c>
-      <c r="B54" t="s">
-        <v>125</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>125</v>
-      </c>
-      <c r="B55" t="s">
-        <v>127</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D55" t="s">
-        <v>129</v>
-      </c>
-      <c r="E55" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>125</v>
-      </c>
-      <c r="B56" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D56" t="s">
-        <v>133</v>
-      </c>
-      <c r="E56" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>125</v>
-      </c>
-      <c r="B57" t="s">
-        <v>135</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>125</v>
-      </c>
-      <c r="B58" t="s">
-        <v>137</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" t="s">
-        <v>138</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>85</v>
-      </c>
-      <c r="B60" t="s">
-        <v>140</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>85</v>
-      </c>
-      <c r="B61" t="s">
-        <v>142</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>85</v>
-      </c>
-      <c r="B62" t="s">
-        <v>144</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>85</v>
-      </c>
-      <c r="B63" t="s">
-        <v>146</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>30</v>
-      </c>
-      <c r="B64" t="s">
-        <v>148</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>85</v>
-      </c>
-      <c r="B65" t="s">
-        <v>150</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>30</v>
-      </c>
-      <c r="B66" t="s">
-        <v>152</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>30</v>
-      </c>
-      <c r="B67" t="s">
-        <v>154</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" t="s">
-        <v>156</v>
-      </c>
-      <c r="C68" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" t="s">
-        <v>158</v>
-      </c>
-      <c r="C69" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" t="s">
-        <v>160</v>
-      </c>
-      <c r="C70" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" t="s">
-        <v>162</v>
-      </c>
-      <c r="C71" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>30</v>
-      </c>
-      <c r="B72" t="s">
-        <v>164</v>
-      </c>
-      <c r="C72" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>85</v>
-      </c>
-      <c r="B73" t="s">
-        <v>166</v>
-      </c>
-      <c r="C73" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>30</v>
-      </c>
-      <c r="B74" t="s">
-        <v>168</v>
-      </c>
-      <c r="C74" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>30</v>
-      </c>
-      <c r="B75" t="s">
-        <v>170</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>30</v>
-      </c>
-      <c r="B76" t="s">
-        <v>172</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>30</v>
-      </c>
-      <c r="B77" t="s">
-        <v>174</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>30</v>
-      </c>
-      <c r="B78" t="s">
-        <v>176</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" t="s">
-        <v>178</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>85</v>
-      </c>
-      <c r="B80" t="s">
-        <v>180</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>85</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>185</v>
+    <row r="83" spans="1:3" ht="15">
+      <c r="A83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15">
+      <c r="A84" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15">
+      <c r="A85" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15">
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15">
+      <c r="A87" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15">
+      <c r="A88" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15">
+      <c r="A89" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15">
+      <c r="A90" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2011,26 +2159,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -2253,40 +2381,34 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}"/>
 </file>
</xml_diff>

<commit_message>
Update PODCAT-795 feature: update site glossary data for global search
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuw5/Documents/GitHub/CCDC-ETL/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6E007E2-8614-4B93-9A29-1005662F26A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4A4EFB-0D69-3B4E-9D7B-18FE55AD0FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22280" windowHeight="14180" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Site glossary'!$A$1:$Z$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Site glossary'!$A$1:$Z$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="212">
   <si>
     <t>Term Category</t>
   </si>
@@ -215,9 +215,6 @@
     <t>FDA</t>
   </si>
   <si>
-    <t>Food and Drug Admistration</t>
-  </si>
-  <si>
     <t>Pediatric Specific</t>
   </si>
   <si>
@@ -542,9 +539,6 @@
     <t>PT</t>
   </si>
   <si>
-    <t>Positrom Emission Tomography (PET)</t>
-  </si>
-  <si>
     <t>M3Cs</t>
   </si>
   <si>
@@ -651,13 +645,43 @@
   </si>
   <si>
     <t>Baylor College of Medicine Advancing Sequencing in Childhood Cancer Care</t>
+  </si>
+  <si>
+    <t>Food and Drug Administration</t>
+  </si>
+  <si>
+    <t>Positron Emission Tomography (PET)</t>
+  </si>
+  <si>
+    <t>MCI</t>
+  </si>
+  <si>
+    <t>Molecular Characterization Initiative</t>
+  </si>
+  <si>
+    <t>OHSU</t>
+  </si>
+  <si>
+    <t>Oregon Health &amp; Science University</t>
+  </si>
+  <si>
+    <t>UCSF</t>
+  </si>
+  <si>
+    <t>University of California, San Francisco</t>
+  </si>
+  <si>
+    <t>MSKCC</t>
+  </si>
+  <si>
+    <t>Memorial Sloan Kettering Cancer Center</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -733,28 +757,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1069,1088 +1089,1131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="99.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="97.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="99.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5" customWidth="1"/>
+    <col min="5" max="5" width="97.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29.1">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29.1">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="1" t="s">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="s">
+      <c r="B24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="2" t="s">
+    </row>
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="43.5">
-      <c r="A29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="29.1">
-      <c r="A30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="57.95">
-      <c r="A31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="E31" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="43.5">
-      <c r="A32" s="1" t="s">
+      <c r="B32" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="29.1">
-      <c r="A33" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
+    </row>
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="2" t="s">
+    </row>
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="2" t="s">
+    </row>
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="2" t="s">
+    </row>
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="2" t="s">
+    </row>
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="2" t="s">
+    </row>
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C43" s="2" t="s">
+    </row>
+    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C45" s="2" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C46" s="2" t="s">
+    </row>
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="2" t="s">
+    </row>
+    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C48" s="2" t="s">
+    </row>
+    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C49" s="2" t="s">
+    </row>
+    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C50" s="2" t="s">
+    </row>
+    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C51" s="2" t="s">
+    </row>
+    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C52" s="2" t="s">
+    </row>
+    <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="29.1">
-      <c r="A53" s="1" t="s">
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="2" t="s">
+    </row>
+    <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>123</v>
+      </c>
+      <c r="B54" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="29.1">
-      <c r="A54" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C54" s="2" t="s">
+    </row>
+    <row r="55" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>125</v>
+      </c>
+      <c r="B55" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="72.599999999999994">
-      <c r="A55" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" t="s">
         <v>129</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" t="s">
         <v>130</v>
       </c>
-      <c r="E55" s="1" t="s">
+    </row>
+    <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="29.1">
-      <c r="A56" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" t="s">
         <v>133</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" t="s">
         <v>134</v>
       </c>
-      <c r="E56" s="1" t="s">
+    </row>
+    <row r="57" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="72.599999999999994">
-      <c r="A57" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C57" s="2" t="s">
+    </row>
+    <row r="58" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="72.599999999999994">
-      <c r="A58" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C58" s="2" t="s">
+    </row>
+    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C59" s="2" t="s">
+    </row>
+    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C60" s="2" t="s">
+    </row>
+    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C61" s="2" t="s">
+    </row>
+    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C62" s="2" t="s">
+    </row>
+    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C63" s="2" t="s">
+    </row>
+    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C64" s="2" t="s">
+    </row>
+    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C65" s="2" t="s">
+    </row>
+    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C66" s="2" t="s">
+    </row>
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C67" s="2" t="s">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" s="1" t="s">
+      <c r="C68" t="s">
         <v>158</v>
       </c>
-      <c r="C68" s="1" t="s">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" t="s">
         <v>160</v>
       </c>
-      <c r="C69" s="1" t="s">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" t="s">
         <v>162</v>
       </c>
-      <c r="C70" s="1" t="s">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" s="1" t="s">
+      <c r="C71" t="s">
         <v>164</v>
       </c>
-      <c r="C71" s="1" t="s">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" t="s">
         <v>166</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C73" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B73" s="1" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" t="s">
         <v>168</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C74" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>30</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75" t="s">
         <v>170</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>30</v>
-      </c>
-      <c r="B75" t="s">
+    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" t="s">
         <v>172</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C76" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>30</v>
-      </c>
-      <c r="B76" t="s">
+    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77" t="s">
         <v>174</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C77" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>30</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" t="s">
         <v>176</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C78" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>30</v>
-      </c>
-      <c r="B78" t="s">
+    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" t="s">
         <v>178</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C79" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" s="1" t="s">
+    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" t="s">
         <v>180</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C80" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B80" s="1" t="s">
+    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C81" s="6" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81" s="7" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C81" s="8" t="s">
+      <c r="C82" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B82" s="9" t="s">
+    <row r="83" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" t="s">
         <v>186</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="C83" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15">
-      <c r="A83" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B83" s="1" t="s">
+    <row r="84" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C84" s="6" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="15">
-      <c r="A84" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B84" s="7" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="C85" s="8" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15">
-      <c r="A85" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B85" s="10" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>84</v>
+      </c>
+      <c r="B86" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C85" s="10" t="s">
+      <c r="C86" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="15">
-      <c r="A86" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B86" s="9" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>84</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C86" s="9" t="s">
+      <c r="C87" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15">
-      <c r="A87" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B87" s="9" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>84</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C87" s="9" t="s">
+      <c r="C88" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15">
-      <c r="A88" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B88" s="9" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>84</v>
+      </c>
+      <c r="B89" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="C88" s="9" t="s">
+      <c r="C89" s="7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15">
-      <c r="A89" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B89" s="9" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>84</v>
+      </c>
+      <c r="B90" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="C89" s="9" t="s">
+      <c r="C90" s="7" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15">
-      <c r="A90" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>203</v>
+    <row r="91" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>84</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>84</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>84</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>84</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z58" xr:uid="{A4DAB4A1-0C2C-4B2F-A024-FF4C6E1E16D8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E58">
-      <sortCondition ref="A1:A58"/>
+  <autoFilter ref="A1:Z1" xr:uid="{A4DAB4A1-0C2C-4B2F-A024-FF4C6E1E16D8}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E1">
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2159,6 +2222,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -2381,15 +2453,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2402,13 +2465,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update PODCAT-795 feature: update site glossary data for global search (#65)
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuw5/Documents/GitHub/CCDC-ETL/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6E007E2-8614-4B93-9A29-1005662F26A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4A4EFB-0D69-3B4E-9D7B-18FE55AD0FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22280" windowHeight="14180" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Site glossary'!$A$1:$Z$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Site glossary'!$A$1:$Z$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="212">
   <si>
     <t>Term Category</t>
   </si>
@@ -215,9 +215,6 @@
     <t>FDA</t>
   </si>
   <si>
-    <t>Food and Drug Admistration</t>
-  </si>
-  <si>
     <t>Pediatric Specific</t>
   </si>
   <si>
@@ -542,9 +539,6 @@
     <t>PT</t>
   </si>
   <si>
-    <t>Positrom Emission Tomography (PET)</t>
-  </si>
-  <si>
     <t>M3Cs</t>
   </si>
   <si>
@@ -651,13 +645,43 @@
   </si>
   <si>
     <t>Baylor College of Medicine Advancing Sequencing in Childhood Cancer Care</t>
+  </si>
+  <si>
+    <t>Food and Drug Administration</t>
+  </si>
+  <si>
+    <t>Positron Emission Tomography (PET)</t>
+  </si>
+  <si>
+    <t>MCI</t>
+  </si>
+  <si>
+    <t>Molecular Characterization Initiative</t>
+  </si>
+  <si>
+    <t>OHSU</t>
+  </si>
+  <si>
+    <t>Oregon Health &amp; Science University</t>
+  </si>
+  <si>
+    <t>UCSF</t>
+  </si>
+  <si>
+    <t>University of California, San Francisco</t>
+  </si>
+  <si>
+    <t>MSKCC</t>
+  </si>
+  <si>
+    <t>Memorial Sloan Kettering Cancer Center</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -733,28 +757,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1069,1088 +1089,1131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="99.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="97.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="99.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5" customWidth="1"/>
+    <col min="5" max="5" width="97.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29.1">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29.1">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1" t="s">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="1" t="s">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="s">
+      <c r="B24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="2" t="s">
+    </row>
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="43.5">
-      <c r="A29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="29.1">
-      <c r="A30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="57.95">
-      <c r="A31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="E31" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="43.5">
-      <c r="A32" s="1" t="s">
+      <c r="B32" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="29.1">
-      <c r="A33" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
+    </row>
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="2" t="s">
+    </row>
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="2" t="s">
+    </row>
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="2" t="s">
+    </row>
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="2" t="s">
+    </row>
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="2" t="s">
+    </row>
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C43" s="2" t="s">
+    </row>
+    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C45" s="2" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C46" s="2" t="s">
+    </row>
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="2" t="s">
+    </row>
+    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C48" s="2" t="s">
+    </row>
+    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C49" s="2" t="s">
+    </row>
+    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C50" s="2" t="s">
+    </row>
+    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C51" s="2" t="s">
+    </row>
+    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C52" s="2" t="s">
+    </row>
+    <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="29.1">
-      <c r="A53" s="1" t="s">
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="2" t="s">
+    </row>
+    <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>123</v>
+      </c>
+      <c r="B54" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="29.1">
-      <c r="A54" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C54" s="2" t="s">
+    </row>
+    <row r="55" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>125</v>
+      </c>
+      <c r="B55" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="72.599999999999994">
-      <c r="A55" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" t="s">
         <v>129</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" t="s">
         <v>130</v>
       </c>
-      <c r="E55" s="1" t="s">
+    </row>
+    <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="29.1">
-      <c r="A56" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" t="s">
         <v>133</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" t="s">
         <v>134</v>
       </c>
-      <c r="E56" s="1" t="s">
+    </row>
+    <row r="57" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="72.599999999999994">
-      <c r="A57" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C57" s="2" t="s">
+    </row>
+    <row r="58" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="72.599999999999994">
-      <c r="A58" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C58" s="2" t="s">
+    </row>
+    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C59" s="2" t="s">
+    </row>
+    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C60" s="2" t="s">
+    </row>
+    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C61" s="2" t="s">
+    </row>
+    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C62" s="2" t="s">
+    </row>
+    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C63" s="2" t="s">
+    </row>
+    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B64" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C64" s="2" t="s">
+    </row>
+    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C65" s="2" t="s">
+    </row>
+    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C66" s="2" t="s">
+    </row>
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C67" s="2" t="s">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B68" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" s="1" t="s">
+      <c r="C68" t="s">
         <v>158</v>
       </c>
-      <c r="C68" s="1" t="s">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" t="s">
         <v>160</v>
       </c>
-      <c r="C69" s="1" t="s">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" t="s">
         <v>162</v>
       </c>
-      <c r="C70" s="1" t="s">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" s="1" t="s">
+      <c r="C71" t="s">
         <v>164</v>
       </c>
-      <c r="C71" s="1" t="s">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" t="s">
         <v>166</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C73" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B73" s="1" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" t="s">
         <v>168</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C74" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>30</v>
-      </c>
-      <c r="B74" t="s">
+    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75" t="s">
         <v>170</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>30</v>
-      </c>
-      <c r="B75" t="s">
+    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" t="s">
         <v>172</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C76" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>30</v>
-      </c>
-      <c r="B76" t="s">
+    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77" t="s">
         <v>174</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C77" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>30</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>30</v>
+      </c>
+      <c r="B78" t="s">
         <v>176</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C78" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>30</v>
-      </c>
-      <c r="B78" t="s">
+    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" t="s">
         <v>178</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C79" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" s="1" t="s">
+    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" t="s">
         <v>180</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C80" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B80" s="1" t="s">
+    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C81" s="6" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81" s="7" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C81" s="8" t="s">
+      <c r="C82" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B82" s="9" t="s">
+    <row r="83" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" t="s">
         <v>186</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="C83" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15">
-      <c r="A83" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B83" s="1" t="s">
+    <row r="84" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C84" s="6" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="15">
-      <c r="A84" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B84" s="7" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="C85" s="8" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15">
-      <c r="A85" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B85" s="10" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>84</v>
+      </c>
+      <c r="B86" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C85" s="10" t="s">
+      <c r="C86" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="15">
-      <c r="A86" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B86" s="9" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>84</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C86" s="9" t="s">
+      <c r="C87" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15">
-      <c r="A87" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B87" s="9" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>84</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C87" s="9" t="s">
+      <c r="C88" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15">
-      <c r="A88" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B88" s="9" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>84</v>
+      </c>
+      <c r="B89" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="C88" s="9" t="s">
+      <c r="C89" s="7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15">
-      <c r="A89" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B89" s="9" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>84</v>
+      </c>
+      <c r="B90" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="C89" s="9" t="s">
+      <c r="C90" s="7" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15">
-      <c r="A90" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>203</v>
+    <row r="91" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>84</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>84</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>84</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>84</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z58" xr:uid="{A4DAB4A1-0C2C-4B2F-A024-FF4C6E1E16D8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E58">
-      <sortCondition ref="A1:A58"/>
+  <autoFilter ref="A1:Z1" xr:uid="{A4DAB4A1-0C2C-4B2F-A024-FF4C6E1E16D8}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E1">
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2159,6 +2222,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -2381,15 +2453,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2402,13 +2465,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
PODCAT-813: Update Glossary Term Category - Image Type
PODCAT-839: re-indexing glossary to DB
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuw5/Documents/GitHub/CCDC-ETL/data_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4A4EFB-0D69-3B4E-9D7B-18FE55AD0FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF84E598-8A41-4E6C-9F33-D2A4EEEA7904}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22280" windowHeight="14180" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="32892" yWindow="792" windowWidth="32664" windowHeight="19500" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Site glossary'!$A$1:$Z$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Site glossary'!$A$1:$Z$97</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="221">
   <si>
     <t>Term Category</t>
   </si>
@@ -215,6 +213,9 @@
     <t>FDA</t>
   </si>
   <si>
+    <t>Food and Drug Administration</t>
+  </si>
+  <si>
     <t>Pediatric Specific</t>
   </si>
   <si>
@@ -500,6 +501,9 @@
     <t xml:space="preserve">Patient-Derived Xenograft and Advanced In Vivo Models </t>
   </si>
   <si>
+    <t>Image Type</t>
+  </si>
+  <si>
     <t>CR</t>
   </si>
   <si>
@@ -539,6 +543,9 @@
     <t>PT</t>
   </si>
   <si>
+    <t>Positron Emission Tomography (PET)</t>
+  </si>
+  <si>
     <t>M3Cs</t>
   </si>
   <si>
@@ -647,12 +654,6 @@
     <t>Baylor College of Medicine Advancing Sequencing in Childhood Cancer Care</t>
   </si>
   <si>
-    <t>Food and Drug Administration</t>
-  </si>
-  <si>
-    <t>Positron Emission Tomography (PET)</t>
-  </si>
-  <si>
     <t>MCI</t>
   </si>
   <si>
@@ -675,6 +676,30 @@
   </si>
   <si>
     <t>Memorial Sloan Kettering Cancer Center</t>
+  </si>
+  <si>
+    <t>PROSPR</t>
+  </si>
+  <si>
+    <t>Population-based Research to Optimize the Screening Process</t>
+  </si>
+  <si>
+    <t>ScPCA</t>
+  </si>
+  <si>
+    <t>Single-cell Pediatric Cancer Atlas</t>
+  </si>
+  <si>
+    <t>GEO</t>
+  </si>
+  <si>
+    <t>Gene Expression Omnibus</t>
+  </si>
+  <si>
+    <t>Any platform, methodology, framework or other software designed for the use of and interpretation of biomedical research data.</t>
+  </si>
+  <si>
+    <t>Analytic Tool</t>
   </si>
 </sst>
 </file>
@@ -757,24 +782,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1089,1131 +1118,1176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="99.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5" customWidth="1"/>
-    <col min="5" max="5" width="97.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="99.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="97.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B74" t="s">
+        <v>171</v>
+      </c>
+      <c r="C74" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" t="s">
+        <v>173</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B76" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" t="s">
+        <v>177</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
+        <v>179</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C89" s="9" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>84</v>
-      </c>
-      <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>84</v>
-      </c>
-      <c r="B36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>84</v>
-      </c>
-      <c r="B40" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" t="s">
-        <v>111</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>84</v>
-      </c>
-      <c r="B48" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>84</v>
-      </c>
-      <c r="B49" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>84</v>
-      </c>
-      <c r="B50" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>84</v>
-      </c>
-      <c r="B51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>84</v>
-      </c>
-      <c r="B52" t="s">
-        <v>121</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>123</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>123</v>
-      </c>
-      <c r="B54" t="s">
-        <v>125</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>125</v>
-      </c>
-      <c r="B55" t="s">
-        <v>127</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D55" t="s">
-        <v>129</v>
-      </c>
-      <c r="E55" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>125</v>
-      </c>
-      <c r="B56" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D56" t="s">
-        <v>133</v>
-      </c>
-      <c r="E56" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>125</v>
-      </c>
-      <c r="B57" t="s">
-        <v>135</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>125</v>
-      </c>
-      <c r="B58" t="s">
-        <v>137</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>84</v>
-      </c>
-      <c r="B59" t="s">
-        <v>139</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>84</v>
-      </c>
-      <c r="B60" t="s">
-        <v>141</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>84</v>
-      </c>
-      <c r="B61" t="s">
-        <v>143</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>84</v>
-      </c>
-      <c r="B62" t="s">
-        <v>145</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>84</v>
-      </c>
-      <c r="B63" t="s">
-        <v>147</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>30</v>
-      </c>
-      <c r="B64" t="s">
-        <v>149</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>84</v>
-      </c>
-      <c r="B65" t="s">
-        <v>151</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>30</v>
-      </c>
-      <c r="B66" t="s">
-        <v>153</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>30</v>
-      </c>
-      <c r="B67" t="s">
-        <v>155</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" t="s">
-        <v>157</v>
-      </c>
-      <c r="C68" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" t="s">
-        <v>159</v>
-      </c>
-      <c r="C69" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" t="s">
-        <v>161</v>
-      </c>
-      <c r="C70" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" t="s">
-        <v>163</v>
-      </c>
-      <c r="C71" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>30</v>
-      </c>
-      <c r="B72" t="s">
-        <v>165</v>
-      </c>
-      <c r="C72" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>84</v>
-      </c>
-      <c r="B73" t="s">
-        <v>166</v>
-      </c>
-      <c r="C73" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>30</v>
-      </c>
-      <c r="B74" t="s">
-        <v>168</v>
-      </c>
-      <c r="C74" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>30</v>
-      </c>
-      <c r="B75" t="s">
-        <v>170</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>30</v>
-      </c>
-      <c r="B76" t="s">
-        <v>172</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>30</v>
-      </c>
-      <c r="B77" t="s">
-        <v>174</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>30</v>
-      </c>
-      <c r="B78" t="s">
-        <v>176</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>84</v>
-      </c>
-      <c r="B79" t="s">
-        <v>178</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>84</v>
-      </c>
-      <c r="B80" t="s">
-        <v>180</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>84</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>84</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>84</v>
-      </c>
-      <c r="B83" t="s">
-        <v>186</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>84</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>84</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>84</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>84</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>84</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>84</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>84</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>84</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>84</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>84</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>84</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>211</v>
+      <c r="B98" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z1" xr:uid="{A4DAB4A1-0C2C-4B2F-A024-FF4C6E1E16D8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E1">
-      <sortCondition ref="A1"/>
+  <autoFilter ref="A1:Z97" xr:uid="{A4DAB4A1-0C2C-4B2F-A024-FF4C6E1E16D8}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E58">
+      <sortCondition ref="A1:A58"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2231,6 +2305,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -2453,17 +2538,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
   <ds:schemaRefs>
@@ -2473,6 +2547,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2489,15 +2580,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
PODCAT-876: Glossary page - new resources abbreviation (CLIC, VPCC, CGC)
Updated Site glossary.xlsx file to contain CLIC, VPCC, CGC
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF84E598-8A41-4E6C-9F33-D2A4EEEA7904}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CDAB790-8FEE-42BD-9117-984DD7237B1A}"/>
   <bookViews>
-    <workbookView xWindow="32892" yWindow="792" windowWidth="32664" windowHeight="19500" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="227">
   <si>
     <t>Term Category</t>
   </si>
@@ -700,13 +700,31 @@
   </si>
   <si>
     <t>Analytic Tool</t>
+  </si>
+  <si>
+    <t>CLIC</t>
+  </si>
+  <si>
+    <t>VPCC</t>
+  </si>
+  <si>
+    <t>Childhood Leukemia International Consortium</t>
+  </si>
+  <si>
+    <t>Victorian Paediatric Cancer Consortium</t>
+  </si>
+  <si>
+    <t>CGC</t>
+  </si>
+  <si>
+    <t>Cancer Genomics Cloud</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -732,6 +750,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -782,7 +807,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -804,6 +829,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1118,23 +1146,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="99.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="97.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="39.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="99.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="97.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1151,7 +1179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1168,7 +1196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1179,7 +1207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1196,7 +1224,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1213,7 +1241,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1230,7 +1258,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1241,7 +1269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1252,7 +1280,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1269,7 +1297,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -1280,7 +1308,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1291,7 +1319,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1302,7 +1330,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1313,7 +1341,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1324,7 +1352,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1335,7 +1363,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1346,7 +1374,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1357,7 +1385,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1368,7 +1396,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1379,7 +1407,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -1390,7 +1418,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1401,7 +1429,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1412,7 +1440,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1423,7 +1451,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
@@ -1434,7 +1462,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>59</v>
       </c>
@@ -1445,7 +1473,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1462,7 +1490,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1479,7 +1507,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1490,7 +1518,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1501,7 +1529,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
@@ -1518,7 +1546,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>24</v>
       </c>
@@ -1535,7 +1563,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>80</v>
       </c>
@@ -1546,7 +1574,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
@@ -1557,7 +1585,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>85</v>
       </c>
@@ -1568,7 +1596,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>85</v>
       </c>
@@ -1579,7 +1607,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>85</v>
       </c>
@@ -1590,7 +1618,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
@@ -1601,7 +1629,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>85</v>
       </c>
@@ -1612,7 +1640,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>85</v>
       </c>
@@ -1623,7 +1651,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>85</v>
       </c>
@@ -1634,7 +1662,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>85</v>
       </c>
@@ -1645,7 +1673,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>85</v>
       </c>
@@ -1656,7 +1684,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>85</v>
       </c>
@@ -1667,7 +1695,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>85</v>
       </c>
@@ -1678,7 +1706,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>85</v>
       </c>
@@ -1689,7 +1717,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>85</v>
       </c>
@@ -1700,7 +1728,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>85</v>
       </c>
@@ -1711,7 +1739,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>85</v>
       </c>
@@ -1722,7 +1750,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>85</v>
       </c>
@@ -1733,7 +1761,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>85</v>
       </c>
@@ -1744,7 +1772,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
@@ -1755,7 +1783,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>85</v>
       </c>
@@ -1766,7 +1794,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>124</v>
       </c>
@@ -1777,7 +1805,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>124</v>
       </c>
@@ -1788,7 +1816,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>126</v>
       </c>
@@ -1805,7 +1833,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>126</v>
       </c>
@@ -1822,7 +1850,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>126</v>
       </c>
@@ -1833,7 +1861,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>126</v>
       </c>
@@ -1844,7 +1872,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>85</v>
       </c>
@@ -1855,7 +1883,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>85</v>
       </c>
@@ -1866,7 +1894,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>85</v>
       </c>
@@ -1877,7 +1905,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>85</v>
       </c>
@@ -1888,7 +1916,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>85</v>
       </c>
@@ -1899,7 +1927,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>30</v>
       </c>
@@ -1910,7 +1938,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>85</v>
       </c>
@@ -1921,7 +1949,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>154</v>
       </c>
@@ -1932,7 +1960,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>154</v>
       </c>
@@ -1943,7 +1971,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>154</v>
       </c>
@@ -1954,7 +1982,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>154</v>
       </c>
@@ -1965,7 +1993,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>154</v>
       </c>
@@ -1976,7 +2004,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>154</v>
       </c>
@@ -1987,7 +2015,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>154</v>
       </c>
@@ -1998,7 +2026,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>85</v>
       </c>
@@ -2009,7 +2037,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>154</v>
       </c>
@@ -2020,7 +2048,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>154</v>
       </c>
@@ -2031,7 +2059,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>154</v>
       </c>
@@ -2042,7 +2070,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>154</v>
       </c>
@@ -2053,7 +2081,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>154</v>
       </c>
@@ -2064,7 +2092,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>85</v>
       </c>
@@ -2075,7 +2103,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>85</v>
       </c>
@@ -2086,7 +2114,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>85</v>
       </c>
@@ -2097,7 +2125,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>85</v>
       </c>
@@ -2108,7 +2136,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>85</v>
       </c>
@@ -2119,7 +2147,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>85</v>
       </c>
@@ -2130,7 +2158,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>85</v>
       </c>
@@ -2141,7 +2169,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
@@ -2152,7 +2180,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
@@ -2163,7 +2191,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
@@ -2174,7 +2202,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -2185,7 +2213,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>85</v>
       </c>
@@ -2196,7 +2224,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>85</v>
       </c>
@@ -2207,7 +2235,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>85</v>
       </c>
@@ -2218,7 +2246,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>85</v>
       </c>
@@ -2229,7 +2257,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>85</v>
       </c>
@@ -2240,7 +2268,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>85</v>
       </c>
@@ -2251,7 +2279,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>85</v>
       </c>
@@ -2262,7 +2290,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>85</v>
       </c>
@@ -2273,7 +2301,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>5</v>
       </c>
@@ -2282,6 +2310,39 @@
       </c>
       <c r="C98" s="2" t="s">
         <v>219</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C101" s="11" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2550,14 +2611,14 @@
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
PODCAT-879: updated glossary excel
PODCAT-879: updated glossary excel
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CDAB790-8FEE-42BD-9117-984DD7237B1A}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6B1D139-5CD4-4107-BB43-0BF3820E7032}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
@@ -807,7 +807,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -823,14 +823,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1148,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1181,120 +1191,108 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>126</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>220</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>85</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>126</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>128</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>129</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1321,13 +1319,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1335,54 +1333,60 @@
         <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>85</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1390,32 +1394,38 @@
         <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>221</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>50</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>52</v>
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1423,110 +1433,98 @@
         <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>59</v>
+        <v>154</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>60</v>
+        <v>155</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>61</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>63</v>
+        <v>85</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>154</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>64</v>
+        <v>157</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>189</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1546,79 +1544,73 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+      <c r="B31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C31" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B35" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
@@ -1629,313 +1621,313 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="1" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" s="1" t="s">
+    <row r="47" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="1" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="1" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" t="s">
+        <v>173</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" t="s">
+        <v>175</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -1943,87 +1935,87 @@
         <v>85</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>153</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>154</v>
+        <v>85</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>154</v>
+        <v>30</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>157</v>
+        <v>41</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>158</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>160</v>
+        <v>85</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>154</v>
+        <v>85</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>164</v>
+        <v>85</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>166</v>
+        <v>85</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>154</v>
+        <v>59</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>168</v>
+        <v>62</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -2031,324 +2023,342 @@
         <v>85</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>170</v>
+        <v>108</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B74" t="s">
-        <v>171</v>
-      </c>
-      <c r="C74" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B75" t="s">
-        <v>173</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B76" t="s">
-        <v>175</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B77" t="s">
-        <v>177</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>178</v>
+        <v>80</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B78" t="s">
-        <v>179</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>180</v>
+        <v>85</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>85</v>
+        <v>154</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B89" t="s">
+        <v>177</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B85" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C85" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B87" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B89" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B92" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B93" s="9" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B96" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>220</v>
+        <v>30</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B99" s="9" t="s">
-        <v>221</v>
+      <c r="B99" s="7" t="s">
+        <v>222</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B100" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+      <c r="B100" t="s">
+        <v>179</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="C101" s="11" t="s">
-        <v>226</v>
+        <v>16</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Z97" xr:uid="{A4DAB4A1-0C2C-4B2F-A024-FF4C6E1E16D8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E58">
-      <sortCondition ref="A1:A58"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E101">
+      <sortCondition ref="B1:B97"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2610,15 +2620,15 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
PODCAT-925: Update ETL to include new glossaries
Updated site glossary excel file
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6B1D139-5CD4-4107-BB43-0BF3820E7032}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D236490-40CF-4615-8994-8A55A7E61AD0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="232">
   <si>
     <t>Term Category</t>
   </si>
@@ -718,6 +718,21 @@
   </si>
   <si>
     <t>Cancer Genomics Cloud</t>
+  </si>
+  <si>
+    <t>Relating to the study of the distribution and determinants of health-related states or events (including disease) in populations, and the application of this study to the control of diseases and other health problems.</t>
+  </si>
+  <si>
+    <t>Epidemiologic</t>
+  </si>
+  <si>
+    <t>Proband</t>
+  </si>
+  <si>
+    <t>Data Element</t>
+  </si>
+  <si>
+    <t>A proband is a person in a family to receive genetic counseling and/or testing for a suspected hereditary risk or diagnosed disease. A proband may or may not be affected with the disease in question. If the value is true, then the case subject may have been diagnosed with the disease under studied. If the value is false, then the case subject is a member of the family of a proband study participant. The proband indicator for the case carries over to a sample taken from a case subject. (Definition based on https://www.cancer.gov/publications/dictionaries/genetics-dictionary/def/proband.)</t>
   </si>
 </sst>
 </file>
@@ -1156,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2353,6 +2368,28 @@
       </c>
       <c r="E101" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2620,16 +2657,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated site glossary file
Updated site glossary file
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D236490-40CF-4615-8994-8A55A7E61AD0}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B38DC1E0-B6F4-4279-853C-327D4B7751F5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="233">
   <si>
     <t>Term Category</t>
   </si>
@@ -732,14 +732,17 @@
     <t>Data Element</t>
   </si>
   <si>
-    <t>A proband is a person in a family to receive genetic counseling and/or testing for a suspected hereditary risk or diagnosed disease. A proband may or may not be affected with the disease in question. If the value is true, then the case subject may have been diagnosed with the disease under studied. If the value is false, then the case subject is a member of the family of a proband study participant. The proband indicator for the case carries over to a sample taken from a case subject. (Definition based on https://www.cancer.gov/publications/dictionaries/genetics-dictionary/def/proband.)</t>
+    <t>A proband is a person in a family to receive genetic counseling and/or testing for a suspected hereditary risk or diagnosed disease. A proband may or may not be affected with the disease in question. If the value is true, then the case subject may have been diagnosed with the disease under studied. If the value is false, then the case subject is a member of the family of a proband study participant. The proband indicator for the case carries over to a sample taken from a case subject.</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/publications/dictionaries/genetics-dictionary/def/proband</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -769,6 +772,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -819,10 +830,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -857,8 +869,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1174,15 +1188,15 @@
   <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="99.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="97.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
@@ -2381,7 +2395,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>230</v>
       </c>
@@ -2390,6 +2404,12 @@
       </c>
       <c r="C103" s="2" t="s">
         <v>231</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E103" s="16" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2398,21 +2418,15 @@
       <sortCondition ref="B1:B97"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="E103" r:id="rId1" xr:uid="{D3DBCC56-4DE9-4D48-A14F-C1E905DF0FDE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
@@ -2421,6 +2435,15 @@
     <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2647,26 +2670,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
PODCAT-925: Update ETL to include new glossaries (#81)
* PODCAT-925: Update ETL to include new glossaries

Updated site glossary excel file

* Updated site glossary file

Updated site glossary file
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6B1D139-5CD4-4107-BB43-0BF3820E7032}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B38DC1E0-B6F4-4279-853C-327D4B7751F5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="233">
   <si>
     <t>Term Category</t>
   </si>
@@ -718,13 +718,31 @@
   </si>
   <si>
     <t>Cancer Genomics Cloud</t>
+  </si>
+  <si>
+    <t>Relating to the study of the distribution and determinants of health-related states or events (including disease) in populations, and the application of this study to the control of diseases and other health problems.</t>
+  </si>
+  <si>
+    <t>Epidemiologic</t>
+  </si>
+  <si>
+    <t>Proband</t>
+  </si>
+  <si>
+    <t>Data Element</t>
+  </si>
+  <si>
+    <t>A proband is a person in a family to receive genetic counseling and/or testing for a suspected hereditary risk or diagnosed disease. A proband may or may not be affected with the disease in question. If the value is true, then the case subject may have been diagnosed with the disease under studied. If the value is false, then the case subject is a member of the family of a proband study participant. The proband indicator for the case carries over to a sample taken from a case subject.</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/publications/dictionaries/genetics-dictionary/def/proband</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -754,6 +772,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -804,10 +830,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -842,8 +869,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1156,18 +1185,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="99.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="97.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
@@ -2355,27 +2384,49 @@
         <v>22</v>
       </c>
     </row>
+    <row r="102" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E103" s="16" t="s">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:Z97" xr:uid="{A4DAB4A1-0C2C-4B2F-A024-FF4C6E1E16D8}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E101">
       <sortCondition ref="B1:B97"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="E103" r:id="rId1" xr:uid="{D3DBCC56-4DE9-4D48-A14F-C1E905DF0FDE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
@@ -2384,6 +2435,15 @@
     <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2610,26 +2670,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Merge from Qa 1.3.4 (#97)
* Update export script

* Update export script to solve automation issue

* Update glossary file
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuw5/Documents/GitHub/CCDC-ETL/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B38DC1E0-B6F4-4279-853C-327D4B7751F5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E902CB-7678-7B42-B8DD-6DA7B2E9E3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="237">
   <si>
     <t>Term Category</t>
   </si>
@@ -736,6 +736,18 @@
   </si>
   <si>
     <t>https://www.cancer.gov/publications/dictionaries/genetics-dictionary/def/proband</t>
+  </si>
+  <si>
+    <t>PPTP</t>
+  </si>
+  <si>
+    <t>Pediatric Preclinical Testing Program</t>
+  </si>
+  <si>
+    <t>DepMap</t>
+  </si>
+  <si>
+    <t>Dependency Map</t>
   </si>
 </sst>
 </file>
@@ -834,39 +846,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -1185,396 +1186,395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="99.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="97.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="97.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="7" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="8" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" t="s">
         <v>120</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B19" s="7" t="s">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>154</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>155</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B25" s="7" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>154</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>157</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>124</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B28" s="1" t="s">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
         <v>189</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="7" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>154</v>
       </c>
       <c r="B31" t="s">
@@ -1584,832 +1584,854 @@
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B32" s="8" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="6" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>150</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" s="7" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" s="1" t="s">
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="7" t="s">
+    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" s="1" t="s">
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
         <v>140</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="1" t="s">
+    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="1" t="s">
+    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
         <v>183</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" s="9" t="s">
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" t="s">
         <v>14</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="1" t="s">
+    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" t="s">
         <v>146</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B46" s="1" t="s">
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>126</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>132</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" t="s">
         <v>134</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="1" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" t="s">
         <v>169</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B49" s="7" t="s">
+    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" s="1" t="s">
+    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" t="s">
         <v>148</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>154</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>159</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B53" s="7" t="s">
+    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B54" s="1" t="s">
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" t="s">
         <v>118</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B55" s="1" t="s">
+    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" t="s">
         <v>98</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B56" s="1" t="s">
+    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>30</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>30</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>39</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>154</v>
       </c>
       <c r="B59" t="s">
         <v>173</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>30</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>51</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B61" s="9" t="s">
+    <row r="61" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B62" s="7" t="s">
+    <row r="62" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>154</v>
       </c>
       <c r="B63" t="s">
         <v>175</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B64" s="1" t="s">
+    <row r="64" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>85</v>
+      </c>
+      <c r="B64" t="s">
         <v>102</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B65" s="1" t="s">
+    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" t="s">
         <v>104</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B66" s="1" t="s">
+    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>85</v>
+      </c>
+      <c r="B66" t="s">
         <v>144</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>30</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
         <v>41</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B68" s="14" t="s">
+    <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>85</v>
+      </c>
+      <c r="B68" t="s">
         <v>152</v>
       </c>
-      <c r="C68" s="15" t="s">
+      <c r="C68" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B69" s="1" t="s">
+    <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69" t="s">
         <v>142</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B70" s="7" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>85</v>
+      </c>
+      <c r="B70" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C70" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B71" s="14" t="s">
+    <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>85</v>
+      </c>
+      <c r="B71" t="s">
         <v>106</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>59</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>62</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B73" s="1" t="s">
+    <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73" t="s">
         <v>108</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B74" s="1" t="s">
+    <row r="74" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" t="s">
         <v>110</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>23</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>24</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>80</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" t="s">
         <v>81</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>80</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" t="s">
         <v>83</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B78" s="1" t="s">
+    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" t="s">
         <v>213</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>154</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" t="s">
         <v>167</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>23</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" t="s">
         <v>3</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>126</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="B81" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C81" s="13" t="s">
+      <c r="C81" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>126</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" t="s">
         <v>138</v>
       </c>
-      <c r="C82" s="15" t="s">
+      <c r="C82" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>23</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" t="s">
         <v>27</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D83" t="s">
         <v>8</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E83" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>124</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B84" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C84" s="13" t="s">
+      <c r="C84" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B85" s="7" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C85" s="5" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>154</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" t="s">
         <v>163</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>154</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" t="s">
         <v>165</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>24</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" t="s">
         <v>77</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D88" t="s">
         <v>8</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E88" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>154</v>
       </c>
       <c r="B89" t="s">
         <v>177</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C89" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B90" s="7" t="s">
+    <row r="90" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>85</v>
+      </c>
+      <c r="B90" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>30</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" t="s">
         <v>53</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B92" s="1" t="s">
+    <row r="92" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>85</v>
+      </c>
+      <c r="B92" t="s">
         <v>112</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B93" s="1" t="s">
+    <row r="93" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>85</v>
+      </c>
+      <c r="B93" t="s">
         <v>114</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B94" s="1" t="s">
+    <row r="94" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>85</v>
+      </c>
+      <c r="B94" t="s">
         <v>116</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B95" s="1" t="s">
+    <row r="95" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>85</v>
+      </c>
+      <c r="B95" t="s">
         <v>181</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C95" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B96" s="7" t="s">
+    <row r="96" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>85</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>154</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" t="s">
         <v>161</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>30</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" t="s">
         <v>55</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C98" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B99" s="7" t="s">
+    <row r="99" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>85</v>
+      </c>
+      <c r="B99" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>154</v>
       </c>
       <c r="B100" t="s">
         <v>179</v>
       </c>
-      <c r="C100" s="6" t="s">
+      <c r="C100" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>16</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" t="s">
         <v>20</v>
       </c>
-      <c r="C101" s="12" t="s">
+      <c r="C101" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D101" t="s">
         <v>14</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="E101" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>5</v>
       </c>
-      <c r="B102" s="14" t="s">
+      <c r="B102" t="s">
         <v>228</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>230</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="B103" t="s">
         <v>229</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" t="s">
         <v>14</v>
       </c>
-      <c r="E103" s="16" t="s">
+      <c r="E103" s="11" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>85</v>
+      </c>
+      <c r="B104" t="s">
+        <v>233</v>
+      </c>
+      <c r="C104" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>85</v>
+      </c>
+      <c r="B105" t="s">
+        <v>235</v>
+      </c>
+      <c r="C105" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2427,26 +2449,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -2669,32 +2671,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59F206A-D323-4CF1-AC59-33871D28A77E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2711,4 +2708,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update global search indices for new resource IDC
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFAFF07D-0905-49CA-B535-CD5A9A629710}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42E81294-C03E-4DA1-A354-D181F120182E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="257">
   <si>
     <t>Term Category</t>
   </si>
@@ -435,12 +435,6 @@
     <t>https://seer.cancer.gov/registries/cancer_registry/index.html</t>
   </si>
   <si>
-    <t>Knowledgebase </t>
-  </si>
-  <si>
-    <t>Biomedical knowledgebases extract, accumulate, organize, annotate, and link the growing body of information that is related to and relies on core datasets. </t>
-  </si>
-  <si>
     <t>NIH ODSS</t>
   </si>
   <si>
@@ -802,6 +796,18 @@
   </si>
   <si>
     <t>Data Repository</t>
+  </si>
+  <si>
+    <t>Knowledgebase</t>
+  </si>
+  <si>
+    <t>Biomedical knowledgebases extract, accumulate, organize, annotate, and link the growing body of information that is related to and relies on core datasets.</t>
+  </si>
+  <si>
+    <t>IDC</t>
+  </si>
+  <si>
+    <t>Imaging Data Commons</t>
   </si>
 </sst>
 </file>
@@ -1244,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:XFD78"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1298,10 +1304,10 @@
         <v>126</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1326,10 +1332,10 @@
         <v>85</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1448,10 +1454,10 @@
         <v>85</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1492,10 +1498,10 @@
         <v>85</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1550,13 +1556,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B24" t="s">
-        <v>154</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1564,21 +1570,21 @@
         <v>85</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1597,10 +1603,10 @@
         <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1608,10 +1614,10 @@
         <v>85</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1633,13 +1639,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B31" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1647,10 +1653,10 @@
         <v>85</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1658,10 +1664,10 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1680,10 +1686,10 @@
         <v>85</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1724,10 +1730,10 @@
         <v>85</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -1735,10 +1741,10 @@
         <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1757,10 +1763,10 @@
         <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -1768,10 +1774,10 @@
         <v>85</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1796,10 +1802,10 @@
         <v>85</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -1818,16 +1824,16 @@
         <v>126</v>
       </c>
       <c r="B47" t="s">
+        <v>253</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D47" t="s">
         <v>132</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="E47" t="s">
         <v>133</v>
-      </c>
-      <c r="D47" t="s">
-        <v>134</v>
-      </c>
-      <c r="E47" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -1835,10 +1841,10 @@
         <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C48" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1846,10 +1852,10 @@
         <v>85</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1868,21 +1874,21 @@
         <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C52" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -1890,10 +1896,10 @@
         <v>85</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1953,13 +1959,13 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B59" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -1978,10 +1984,10 @@
         <v>85</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -1989,21 +1995,21 @@
         <v>85</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B63" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -2033,10 +2039,10 @@
         <v>85</v>
       </c>
       <c r="B66" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -2055,10 +2061,10 @@
         <v>85</v>
       </c>
       <c r="B68" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -2066,10 +2072,10 @@
         <v>85</v>
       </c>
       <c r="B69" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -2077,10 +2083,10 @@
         <v>85</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -2162,13 +2168,13 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B78" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C78" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2187,10 +2193,10 @@
         <v>126</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -2198,10 +2204,10 @@
         <v>126</v>
       </c>
       <c r="B81" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
@@ -2237,32 +2243,32 @@
         <v>85</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B85" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C85" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B86" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C86" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="58" x14ac:dyDescent="0.35">
@@ -2284,13 +2290,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B88" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
@@ -2298,10 +2304,10 @@
         <v>85</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
@@ -2353,10 +2359,10 @@
         <v>85</v>
       </c>
       <c r="B94" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
@@ -2364,21 +2370,21 @@
         <v>85</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B96" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C96" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
@@ -2397,21 +2403,21 @@
         <v>85</v>
       </c>
       <c r="B98" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B99" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
@@ -2436,27 +2442,27 @@
         <v>5</v>
       </c>
       <c r="B101" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B102" t="s">
+        <v>224</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="D102" t="s">
         <v>14</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
@@ -2464,10 +2470,10 @@
         <v>85</v>
       </c>
       <c r="B103" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
@@ -2475,10 +2481,10 @@
         <v>85</v>
       </c>
       <c r="B104" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
@@ -2486,10 +2492,10 @@
         <v>85</v>
       </c>
       <c r="B105" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
@@ -2497,10 +2503,10 @@
         <v>30</v>
       </c>
       <c r="B106" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
@@ -2508,10 +2514,10 @@
         <v>85</v>
       </c>
       <c r="B107" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
@@ -2519,10 +2525,10 @@
         <v>85</v>
       </c>
       <c r="B108" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -2530,16 +2536,16 @@
         <v>5</v>
       </c>
       <c r="B109" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D109" t="s">
         <v>14</v>
       </c>
       <c r="E109" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
@@ -2547,16 +2553,16 @@
         <v>126</v>
       </c>
       <c r="B110" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D110" t="s">
         <v>14</v>
       </c>
       <c r="E110" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
@@ -2564,10 +2570,10 @@
         <v>85</v>
       </c>
       <c r="B111" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
@@ -2575,10 +2581,10 @@
         <v>85</v>
       </c>
       <c r="B112" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
@@ -2586,10 +2592,21 @@
         <v>85</v>
       </c>
       <c r="B113" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>85</v>
+      </c>
+      <c r="B114" t="s">
+        <v>255</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -2607,14 +2624,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2853,39 +2868,56 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A423FFE3-1836-40F2-AA2D-E6E0D3E22438}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A423FFE3-1836-40F2-AA2D-E6E0D3E22438}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add new site glossary file
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27002"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43723CE2-BD96-4FDB-B619-D95EA49C9875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C980E25C-B7F9-4754-A147-B0E985A87EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="259">
   <si>
     <t>Term Category</t>
   </si>
@@ -808,6 +808,12 @@
   </si>
   <si>
     <t>Imaging Data Commons</t>
+  </si>
+  <si>
+    <t>OSE</t>
+  </si>
+  <si>
+    <t>Osteosarcoma Explorer</t>
   </si>
 </sst>
 </file>
@@ -1246,17 +1252,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="99.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="97.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1295,7 +1301,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.9">
+    <row r="3" spans="1:5" ht="29.1">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1356,7 +1362,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="72">
+    <row r="8" spans="1:5" ht="72.599999999999994">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1539,7 +1545,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.15">
+    <row r="23" spans="1:5" ht="43.5">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1583,7 +1589,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="28.9">
+    <row r="27" spans="1:5" ht="29.1">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -1616,7 +1622,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="28.9">
+    <row r="30" spans="1:5" ht="29.1">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="28.9">
+    <row r="44" spans="1:5" ht="29.1">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -1815,7 +1821,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="28.9">
+    <row r="47" spans="1:5" ht="29.1">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2129,7 +2135,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="43.15">
+    <row r="75" spans="1:3" ht="43.5">
       <c r="A75" t="s">
         <v>171</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="43.15">
+    <row r="76" spans="1:3" ht="43.5">
       <c r="A76" t="s">
         <v>173</v>
       </c>
@@ -2151,7 +2157,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="28.9">
+    <row r="77" spans="1:3" ht="29.1">
       <c r="A77" t="s">
         <v>173</v>
       </c>
@@ -2173,7 +2179,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="28.9">
+    <row r="79" spans="1:3" ht="29.1">
       <c r="A79" t="s">
         <v>171</v>
       </c>
@@ -2184,7 +2190,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="72">
+    <row r="80" spans="1:3" ht="72.599999999999994">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -2195,7 +2201,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="72">
+    <row r="81" spans="1:5" ht="72.599999999999994">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -2223,7 +2229,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="28.9">
+    <row r="83" spans="1:5" ht="29.1">
       <c r="A83" t="s">
         <v>70</v>
       </c>
@@ -2267,7 +2273,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="57.6">
+    <row r="87" spans="1:5" ht="57.95">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -2433,7 +2439,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="28.9">
+    <row r="101" spans="1:5" ht="29.1">
       <c r="A101" t="s">
         <v>53</v>
       </c>
@@ -2444,7 +2450,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="72">
+    <row r="102" spans="1:5" ht="72.599999999999994">
       <c r="A102" t="s">
         <v>227</v>
       </c>
@@ -2527,7 +2533,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="28.9">
+    <row r="109" spans="1:5" ht="29.1">
       <c r="A109" t="s">
         <v>53</v>
       </c>
@@ -2544,7 +2550,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="72">
+    <row r="110" spans="1:5" ht="72.599999999999994">
       <c r="A110" t="s">
         <v>10</v>
       </c>
@@ -2603,6 +2609,17 @@
       </c>
       <c r="C114" s="1" t="s">
         <v>256</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>17</v>
+      </c>
+      <c r="B115" t="s">
+        <v>257</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2620,6 +2637,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="23634515e2fd75be5bfad7623104c70a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="305374924f9daf7f55b4f039a6f85780" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -2854,28 +2891,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A423FFE3-1836-40F2-AA2D-E6E0D3E22438}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2883,5 +2900,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A423FFE3-1836-40F2-AA2D-E6E0D3E22438}"/>
 </file>
</xml_diff>

<commit_message>
Add new site glossary file (#125)
Co-authored-by: Wei Yu <ywwei85@gmail.com>
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27002"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43723CE2-BD96-4FDB-B619-D95EA49C9875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C980E25C-B7F9-4754-A147-B0E985A87EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="259">
   <si>
     <t>Term Category</t>
   </si>
@@ -808,6 +808,12 @@
   </si>
   <si>
     <t>Imaging Data Commons</t>
+  </si>
+  <si>
+    <t>OSE</t>
+  </si>
+  <si>
+    <t>Osteosarcoma Explorer</t>
   </si>
 </sst>
 </file>
@@ -1246,17 +1252,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="99.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="97.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1295,7 +1301,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.9">
+    <row r="3" spans="1:5" ht="29.1">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1356,7 +1362,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="72">
+    <row r="8" spans="1:5" ht="72.599999999999994">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1539,7 +1545,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.15">
+    <row r="23" spans="1:5" ht="43.5">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1583,7 +1589,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="28.9">
+    <row r="27" spans="1:5" ht="29.1">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -1616,7 +1622,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="28.9">
+    <row r="30" spans="1:5" ht="29.1">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="28.9">
+    <row r="44" spans="1:5" ht="29.1">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -1815,7 +1821,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="28.9">
+    <row r="47" spans="1:5" ht="29.1">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2129,7 +2135,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="43.15">
+    <row r="75" spans="1:3" ht="43.5">
       <c r="A75" t="s">
         <v>171</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="43.15">
+    <row r="76" spans="1:3" ht="43.5">
       <c r="A76" t="s">
         <v>173</v>
       </c>
@@ -2151,7 +2157,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="28.9">
+    <row r="77" spans="1:3" ht="29.1">
       <c r="A77" t="s">
         <v>173</v>
       </c>
@@ -2173,7 +2179,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="28.9">
+    <row r="79" spans="1:3" ht="29.1">
       <c r="A79" t="s">
         <v>171</v>
       </c>
@@ -2184,7 +2190,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="72">
+    <row r="80" spans="1:3" ht="72.599999999999994">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -2195,7 +2201,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="72">
+    <row r="81" spans="1:5" ht="72.599999999999994">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -2223,7 +2229,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="28.9">
+    <row r="83" spans="1:5" ht="29.1">
       <c r="A83" t="s">
         <v>70</v>
       </c>
@@ -2267,7 +2273,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="57.6">
+    <row r="87" spans="1:5" ht="57.95">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -2433,7 +2439,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="28.9">
+    <row r="101" spans="1:5" ht="29.1">
       <c r="A101" t="s">
         <v>53</v>
       </c>
@@ -2444,7 +2450,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="72">
+    <row r="102" spans="1:5" ht="72.599999999999994">
       <c r="A102" t="s">
         <v>227</v>
       </c>
@@ -2527,7 +2533,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="28.9">
+    <row r="109" spans="1:5" ht="29.1">
       <c r="A109" t="s">
         <v>53</v>
       </c>
@@ -2544,7 +2550,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="72">
+    <row r="110" spans="1:5" ht="72.599999999999994">
       <c r="A110" t="s">
         <v>10</v>
       </c>
@@ -2603,6 +2609,17 @@
       </c>
       <c r="C114" s="1" t="s">
         <v>256</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>17</v>
+      </c>
+      <c r="B115" t="s">
+        <v>257</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2620,6 +2637,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="23634515e2fd75be5bfad7623104c70a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="305374924f9daf7f55b4f039a6f85780" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -2854,28 +2891,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A423FFE3-1836-40F2-AA2D-E6E0D3E22438}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2883,5 +2900,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A423FFE3-1836-40F2-AA2D-E6E0D3E22438}"/>
 </file>
</xml_diff>

<commit_message>
Update site glossary (#134)
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27321"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C70A91F8-CEF2-4367-838D-DD975BB8310B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1C4C280-E5A2-498D-8584-46E4997D247B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="273">
   <si>
     <t>Term Category</t>
   </si>
@@ -850,6 +850,12 @@
   </si>
   <si>
     <t>Pediatric Preclinical In Vivo Testing Consortium</t>
+  </si>
+  <si>
+    <t>GENIE</t>
+  </si>
+  <si>
+    <t>Genomics Evidence Neoplasia Information Exchange</t>
   </si>
 </sst>
 </file>
@@ -1288,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -2722,6 +2728,17 @@
       </c>
       <c r="C121" s="1" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>17</v>
+      </c>
+      <c r="B122" t="s">
+        <v>271</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -2739,15 +2756,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
@@ -2758,9 +2766,18 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="23634515e2fd75be5bfad7623104c70a">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="305374924f9daf7f55b4f039a6f85780" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1061af385f784bd525987ba0873cd3dd">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6d926a13f4595f889af4c5a97ebe0f1" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
     <xsd:import namespace="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
     <xsd:element name="properties">
@@ -2783,6 +2800,7 @@
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2850,6 +2868,11 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="22" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="23" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -2994,13 +3017,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A423FFE3-1836-40F2-AA2D-E6E0D3E22438}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EAF87E7-5A4A-4BD2-B913-58D76814E19A}"/>
 </file>
</xml_diff>

<commit_message>
Updated site glossary doc
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0051A357-B2B8-492D-A5DF-713868BBFD43}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E57A5F25-5F68-4F35-B9B0-605A4F843270}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="287">
   <si>
     <t>Term Category</t>
   </si>
@@ -892,6 +892,12 @@
   </si>
   <si>
     <t>DCEG</t>
+  </si>
+  <si>
+    <t>ecDNA</t>
+  </si>
+  <si>
+    <t>Circular Extrachromosomal DNA</t>
   </si>
 </sst>
 </file>
@@ -1340,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1666,7 +1672,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -1887,7 +1893,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>126</v>
       </c>
@@ -2851,6 +2857,17 @@
       </c>
       <c r="C128" s="1" t="s">
         <v>283</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>85</v>
+      </c>
+      <c r="B129" t="s">
+        <v>285</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2868,7 +2885,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1061af385f784bd525987ba0873cd3dd">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="45d1a909a05463e745eea5a4ca1d742b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6d926a13f4595f889af4c5a97ebe0f1" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
     <xsd:import namespace="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
@@ -3109,15 +3126,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
@@ -3128,8 +3136,17 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EAF87E7-5A4A-4BD2-B913-58D76814E19A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE669BE3-DCA4-4A66-AC51-61E254098965}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -3148,26 +3165,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated site glossary doc (#149)
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0051A357-B2B8-492D-A5DF-713868BBFD43}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E57A5F25-5F68-4F35-B9B0-605A4F843270}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="287">
   <si>
     <t>Term Category</t>
   </si>
@@ -892,6 +892,12 @@
   </si>
   <si>
     <t>DCEG</t>
+  </si>
+  <si>
+    <t>ecDNA</t>
+  </si>
+  <si>
+    <t>Circular Extrachromosomal DNA</t>
   </si>
 </sst>
 </file>
@@ -1340,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1666,7 +1672,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -1887,7 +1893,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>126</v>
       </c>
@@ -2851,6 +2857,17 @@
       </c>
       <c r="C128" s="1" t="s">
         <v>283</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>85</v>
+      </c>
+      <c r="B129" t="s">
+        <v>285</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2868,7 +2885,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1061af385f784bd525987ba0873cd3dd">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="45d1a909a05463e745eea5a4ca1d742b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6d926a13f4595f889af4c5a97ebe0f1" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
     <xsd:import namespace="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
@@ -3109,15 +3126,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
@@ -3128,8 +3136,17 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EAF87E7-5A4A-4BD2-B913-58D76814E19A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE669BE3-DCA4-4A66-AC51-61E254098965}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -3148,26 +3165,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated site glossary doc (#149) (#151)
Co-authored-by: Ruoxi Zhang <116577061+RuoxiZhang08@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0051A357-B2B8-492D-A5DF-713868BBFD43}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E57A5F25-5F68-4F35-B9B0-605A4F843270}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Site glossary" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="287">
   <si>
     <t>Term Category</t>
   </si>
@@ -892,6 +892,12 @@
   </si>
   <si>
     <t>DCEG</t>
+  </si>
+  <si>
+    <t>ecDNA</t>
+  </si>
+  <si>
+    <t>Circular Extrachromosomal DNA</t>
   </si>
 </sst>
 </file>
@@ -1340,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1666,7 +1672,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>124</v>
       </c>
@@ -1887,7 +1893,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>126</v>
       </c>
@@ -2851,6 +2857,17 @@
       </c>
       <c r="C128" s="1" t="s">
         <v>283</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>85</v>
+      </c>
+      <c r="B129" t="s">
+        <v>285</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2868,7 +2885,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1061af385f784bd525987ba0873cd3dd">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="45d1a909a05463e745eea5a4ca1d742b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6d926a13f4595f889af4c5a97ebe0f1" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
     <xsd:import namespace="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
@@ -3109,15 +3126,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
@@ -3128,8 +3136,17 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EAF87E7-5A4A-4BD2-B913-58D76814E19A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE669BE3-DCA4-4A66-AC51-61E254098965}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -3148,26 +3165,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7554B1E-EA5B-4036-8BEB-CEB54DFFA990}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
PODCAT-1669: Updated Site Glossary 1.5.6
</commit_message>
<xml_diff>
--- a/data_files/Site glossary.xlsx
+++ b/data_files/Site glossary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E57A5F25-5F68-4F35-B9B0-605A4F843270}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="13_ncr:1_{CD305CA4-F6E6-494C-8D70-07316997D1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30E0CF6A-27B9-401F-AEF6-0E6657FAAEB3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4110CF64-F05A-4DD9-960E-BC3FCD1C46EE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="289">
   <si>
     <t>Term Category</t>
   </si>
@@ -898,6 +898,12 @@
   </si>
   <si>
     <t>Circular Extrachromosomal DNA</t>
+  </si>
+  <si>
+    <t>FAPTP</t>
+  </si>
+  <si>
+    <t>Florida Association of Pediatric Tumor Programs</t>
   </si>
 </sst>
 </file>
@@ -1346,10 +1352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69208F35-5666-473F-97EF-CB7A96B85984}">
-  <dimension ref="A1:E129"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2868,6 +2874,17 @@
       </c>
       <c r="C129" s="1" t="s">
         <v>286</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>85</v>
+      </c>
+      <c r="B130" t="s">
+        <v>287</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2885,8 +2902,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="45d1a909a05463e745eea5a4ca1d742b">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6d926a13f4595f889af4c5a97ebe0f1" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d2768cdbde6492a0492d94561974b69">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8301a1e8c200ff5d9a28910b74393c39" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
     <xsd:import namespace="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
     <xsd:element name="properties">
@@ -2910,6 +2938,7 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2980,6 +3009,11 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceSearchProperties" ma:index="23" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="24" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
@@ -3125,17 +3159,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3146,39 +3169,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE669BE3-DCA4-4A66-AC51-61E254098965}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
     <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13521947-7B63-4043-9A52-D2F3EDCA31C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CAE602F-C18F-4F58-99E8-C3206052EF37}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>